<commit_message>
Updated questions and lists
</commit_message>
<xml_diff>
--- a/lists/lists.rs.xlsx
+++ b/lists/lists.rs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="2895" windowWidth="15600" windowHeight="5190" activeTab="4"/>
+    <workbookView xWindow="210" yWindow="2895" windowWidth="15600" windowHeight="5190" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="fractions" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1810" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1899" uniqueCount="341">
   <si>
     <t>RAZRED</t>
   </si>
@@ -1006,12 +1006,60 @@
   <si>
     <t>Zapremina kvadra</t>
   </si>
+  <si>
+    <t>Rogljasta i obla tela</t>
+  </si>
+  <si>
+    <t>numb.145</t>
+  </si>
+  <si>
+    <t>Mreža</t>
+  </si>
+  <si>
+    <t>Elementi i osobine</t>
+  </si>
+  <si>
+    <t>Kvadar i kocka</t>
+  </si>
+  <si>
+    <t>Prava</t>
+  </si>
+  <si>
+    <t>Uzajamni položaj pravih</t>
+  </si>
+  <si>
+    <t>Ugao</t>
+  </si>
+  <si>
+    <t>Vrste uglova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojam, elementi </t>
+  </si>
+  <si>
+    <t>Kružnica i krug</t>
+  </si>
+  <si>
+    <t>Pravougaonik, kvadrat</t>
+  </si>
+  <si>
+    <t>meas.3</t>
+  </si>
+  <si>
+    <t>Obim kvadrata</t>
+  </si>
+  <si>
+    <t>Trougao</t>
+  </si>
+  <si>
+    <t>Pojam, elementi I  vrste</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1036,6 +1084,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1133,7 +1188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1321,6 +1376,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1329,22 +1386,14 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFCC"/>
       <color rgb="FFCCFFFF"/>
       <color rgb="FF99FFCC"/>
-      <color rgb="FFFFFFCC"/>
       <color rgb="FFCCECFF"/>
       <color rgb="FF99CCFF"/>
       <color rgb="FFCCFFCC"/>
     </mruColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1636,7 +1685,7 @@
   <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I82" sqref="I82"/>
     </sheetView>
   </sheetViews>
@@ -3678,11 +3727,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD23"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4136,7 +4185,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="42">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="42">
         <v>1</v>
@@ -4145,25 +4194,25 @@
         <v>2</v>
       </c>
       <c r="E17" s="42">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F17" s="43" t="s">
         <v>249</v>
       </c>
-      <c r="G17" s="44" t="s">
-        <v>189</v>
-      </c>
-      <c r="H17" s="45" t="s">
-        <v>79</v>
+      <c r="G17" s="74" t="s">
+        <v>336</v>
+      </c>
+      <c r="H17" s="73" t="s">
+        <v>334</v>
       </c>
       <c r="I17" s="42"/>
     </row>
-    <row r="18" spans="1:9" s="46" customFormat="1">
+    <row r="18" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
       <c r="A18" s="42">
         <v>3</v>
       </c>
       <c r="B18" s="42">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="42">
         <v>1</v>
@@ -4172,7 +4221,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="42">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F18" s="43" t="s">
         <v>249</v>
@@ -4180,8 +4229,8 @@
       <c r="G18" s="44" t="s">
         <v>189</v>
       </c>
-      <c r="H18" s="44" t="s">
-        <v>80</v>
+      <c r="H18" s="45" t="s">
+        <v>79</v>
       </c>
       <c r="I18" s="42"/>
     </row>
@@ -4190,7 +4239,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="42">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="42">
         <v>1</v>
@@ -4199,7 +4248,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="42">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F19" s="43" t="s">
         <v>249</v>
@@ -4208,19 +4257,19 @@
         <v>189</v>
       </c>
       <c r="H19" s="44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I19" s="42"/>
     </row>
-    <row r="20" spans="1:9" s="46" customFormat="1" ht="18" customHeight="1">
+    <row r="20" spans="1:9" s="46" customFormat="1">
       <c r="A20" s="42">
         <v>3</v>
       </c>
       <c r="B20" s="42">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="43">
         <v>2</v>
@@ -4232,19 +4281,19 @@
         <v>249</v>
       </c>
       <c r="G20" s="44" t="s">
-        <v>190</v>
-      </c>
-      <c r="H20" s="45" t="s">
-        <v>82</v>
+        <v>189</v>
+      </c>
+      <c r="H20" s="44" t="s">
+        <v>81</v>
       </c>
       <c r="I20" s="42"/>
     </row>
-    <row r="21" spans="1:9" s="46" customFormat="1" ht="17.25" customHeight="1">
+    <row r="21" spans="1:9" s="46" customFormat="1" ht="18" customHeight="1">
       <c r="A21" s="42">
         <v>3</v>
       </c>
       <c r="B21" s="42">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="42">
         <v>0</v>
@@ -4266,12 +4315,12 @@
       </c>
       <c r="I21" s="42"/>
     </row>
-    <row r="22" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+    <row r="22" spans="1:9" s="46" customFormat="1" ht="17.25" customHeight="1">
       <c r="A22" s="42">
         <v>3</v>
       </c>
       <c r="B22" s="42">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" s="42">
         <v>0</v>
@@ -4293,225 +4342,1044 @@
       </c>
       <c r="I22" s="42"/>
     </row>
-    <row r="23" spans="1:9" s="13" customFormat="1">
-      <c r="A23" s="9">
-        <v>1</v>
-      </c>
-      <c r="B23" s="9">
+    <row r="23" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="A23" s="42">
+        <v>3</v>
+      </c>
+      <c r="B23" s="42">
+        <v>22</v>
+      </c>
+      <c r="C23" s="42">
+        <v>0</v>
+      </c>
+      <c r="D23" s="43">
+        <v>2</v>
+      </c>
+      <c r="E23" s="42">
+        <v>1</v>
+      </c>
+      <c r="F23" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G23" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="H23" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="I23" s="42"/>
+    </row>
+    <row r="24" spans="1:9" s="53" customFormat="1" ht="15" customHeight="1">
+      <c r="A24" s="50">
+        <v>4</v>
+      </c>
+      <c r="B24" s="50">
+        <v>23</v>
+      </c>
+      <c r="C24" s="50">
+        <v>0</v>
+      </c>
+      <c r="D24" s="51">
+        <v>2</v>
+      </c>
+      <c r="E24" s="50">
+        <v>1</v>
+      </c>
+      <c r="F24" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="G24" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="H24" s="56" t="s">
+        <v>325</v>
+      </c>
+      <c r="I24" s="50">
         <v>43</v>
       </c>
-      <c r="C23" s="9">
+    </row>
+    <row r="25" spans="1:9" s="53" customFormat="1" ht="15" customHeight="1">
+      <c r="A25" s="50">
+        <v>4</v>
+      </c>
+      <c r="B25" s="50">
+        <v>24</v>
+      </c>
+      <c r="C25" s="50">
+        <v>1</v>
+      </c>
+      <c r="D25" s="51">
+        <v>2</v>
+      </c>
+      <c r="E25" s="50">
+        <v>1</v>
+      </c>
+      <c r="F25" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="G25" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="H25" s="56" t="s">
+        <v>325</v>
+      </c>
+      <c r="I25" s="50">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="53" customFormat="1" ht="15" customHeight="1">
+      <c r="A26" s="50">
+        <v>4</v>
+      </c>
+      <c r="B26" s="50">
+        <v>25</v>
+      </c>
+      <c r="C26" s="50">
+        <v>1</v>
+      </c>
+      <c r="D26" s="51">
+        <v>2</v>
+      </c>
+      <c r="E26" s="50">
+        <v>1</v>
+      </c>
+      <c r="F26" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="G26" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="H26" s="56" t="s">
+        <v>325</v>
+      </c>
+      <c r="I26" s="50" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="53" customFormat="1" ht="15" customHeight="1">
+      <c r="A27" s="50">
+        <v>4</v>
+      </c>
+      <c r="B27" s="50">
+        <v>26</v>
+      </c>
+      <c r="C27" s="50">
+        <v>1</v>
+      </c>
+      <c r="D27" s="51">
+        <v>2</v>
+      </c>
+      <c r="E27" s="50">
+        <v>1</v>
+      </c>
+      <c r="F27" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="G27" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="H27" s="56" t="s">
+        <v>325</v>
+      </c>
+      <c r="I27" s="50">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="53" customFormat="1" ht="15" customHeight="1">
+      <c r="A28" s="50">
+        <v>4</v>
+      </c>
+      <c r="B28" s="50">
+        <v>27</v>
+      </c>
+      <c r="C28" s="50">
+        <v>1</v>
+      </c>
+      <c r="D28" s="51">
+        <v>2</v>
+      </c>
+      <c r="E28" s="50">
+        <v>1</v>
+      </c>
+      <c r="F28" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="G28" s="56" t="s">
+        <v>329</v>
+      </c>
+      <c r="H28" s="56" t="s">
+        <v>327</v>
+      </c>
+      <c r="I28" s="50"/>
+    </row>
+    <row r="29" spans="1:9" s="53" customFormat="1" ht="15" customHeight="1">
+      <c r="A29" s="50">
+        <v>4</v>
+      </c>
+      <c r="B29" s="50">
+        <v>28</v>
+      </c>
+      <c r="C29" s="50">
+        <v>1</v>
+      </c>
+      <c r="D29" s="51">
+        <v>2</v>
+      </c>
+      <c r="E29" s="50">
+        <v>1</v>
+      </c>
+      <c r="F29" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="G29" s="56" t="s">
+        <v>329</v>
+      </c>
+      <c r="H29" s="56" t="s">
+        <v>328</v>
+      </c>
+      <c r="I29" s="50">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="53" customFormat="1" ht="15" customHeight="1">
+      <c r="A30" s="50">
+        <v>4</v>
+      </c>
+      <c r="B30" s="50">
+        <v>29</v>
+      </c>
+      <c r="C30" s="50">
         <v>0</v>
       </c>
-      <c r="D23" s="10">
-        <v>1</v>
-      </c>
-      <c r="E23" s="9">
-        <v>1</v>
-      </c>
-      <c r="F23" s="10" t="s">
+      <c r="D30" s="51">
+        <v>2</v>
+      </c>
+      <c r="E30" s="50">
+        <v>1</v>
+      </c>
+      <c r="F30" s="51" t="s">
         <v>249</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G30" s="56" t="s">
+        <v>329</v>
+      </c>
+      <c r="H30" s="56" t="s">
+        <v>327</v>
+      </c>
+      <c r="I30" s="50">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="A31" s="42">
+        <v>3</v>
+      </c>
+      <c r="B31" s="42">
+        <v>30</v>
+      </c>
+      <c r="C31" s="42">
+        <v>1</v>
+      </c>
+      <c r="D31" s="43">
+        <v>1</v>
+      </c>
+      <c r="E31" s="42">
+        <v>1</v>
+      </c>
+      <c r="F31" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G31" s="73" t="s">
+        <v>330</v>
+      </c>
+      <c r="H31" s="73" t="s">
+        <v>331</v>
+      </c>
+      <c r="I31" s="42"/>
+    </row>
+    <row r="32" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="A32" s="42">
+        <v>3</v>
+      </c>
+      <c r="B32" s="42">
+        <v>31</v>
+      </c>
+      <c r="C32" s="42">
+        <v>1</v>
+      </c>
+      <c r="D32" s="43">
+        <v>1</v>
+      </c>
+      <c r="E32" s="42">
+        <v>1</v>
+      </c>
+      <c r="F32" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G32" s="73" t="s">
+        <v>330</v>
+      </c>
+      <c r="H32" s="73" t="s">
+        <v>331</v>
+      </c>
+      <c r="I32" s="42">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="A33" s="42">
+        <v>3</v>
+      </c>
+      <c r="B33" s="42">
+        <v>32</v>
+      </c>
+      <c r="C33" s="42">
+        <v>0</v>
+      </c>
+      <c r="D33" s="43">
+        <v>1</v>
+      </c>
+      <c r="E33" s="42">
+        <v>1</v>
+      </c>
+      <c r="F33" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G33" s="73" t="s">
+        <v>332</v>
+      </c>
+      <c r="H33" s="73" t="s">
+        <v>334</v>
+      </c>
+      <c r="I33" s="42">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="A34" s="42">
+        <v>3</v>
+      </c>
+      <c r="B34" s="42">
+        <v>33</v>
+      </c>
+      <c r="C34" s="42">
+        <v>0</v>
+      </c>
+      <c r="D34" s="43">
+        <v>1</v>
+      </c>
+      <c r="E34" s="42">
+        <v>1</v>
+      </c>
+      <c r="F34" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G34" s="73" t="s">
+        <v>332</v>
+      </c>
+      <c r="H34" s="73" t="s">
+        <v>334</v>
+      </c>
+      <c r="I34" s="42"/>
+    </row>
+    <row r="35" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="A35" s="42">
+        <v>3</v>
+      </c>
+      <c r="B35" s="42">
+        <v>34</v>
+      </c>
+      <c r="C35" s="42">
+        <v>0</v>
+      </c>
+      <c r="D35" s="43">
+        <v>1</v>
+      </c>
+      <c r="E35" s="42">
+        <v>1</v>
+      </c>
+      <c r="F35" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G35" s="73" t="s">
+        <v>332</v>
+      </c>
+      <c r="H35" s="73" t="s">
+        <v>334</v>
+      </c>
+      <c r="I35" s="42">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="A36" s="42">
+        <v>3</v>
+      </c>
+      <c r="B36" s="42">
+        <v>35</v>
+      </c>
+      <c r="C36" s="42">
+        <v>1</v>
+      </c>
+      <c r="D36" s="43">
+        <v>1</v>
+      </c>
+      <c r="E36" s="42">
+        <v>1</v>
+      </c>
+      <c r="F36" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G36" s="73" t="s">
+        <v>332</v>
+      </c>
+      <c r="H36" s="73" t="s">
+        <v>334</v>
+      </c>
+      <c r="I36" s="42">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="A37" s="42">
+        <v>3</v>
+      </c>
+      <c r="B37" s="42">
+        <v>36</v>
+      </c>
+      <c r="C37" s="42">
+        <v>1</v>
+      </c>
+      <c r="D37" s="43">
+        <v>1</v>
+      </c>
+      <c r="E37" s="42">
+        <v>1</v>
+      </c>
+      <c r="F37" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G37" s="73" t="s">
+        <v>332</v>
+      </c>
+      <c r="H37" s="73" t="s">
+        <v>333</v>
+      </c>
+      <c r="I37" s="42"/>
+    </row>
+    <row r="38" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="A38" s="42">
+        <v>3</v>
+      </c>
+      <c r="B38" s="42">
+        <v>37</v>
+      </c>
+      <c r="C38" s="42">
+        <v>1</v>
+      </c>
+      <c r="D38" s="43">
+        <v>1</v>
+      </c>
+      <c r="E38" s="42">
+        <v>2</v>
+      </c>
+      <c r="F38" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G38" s="73" t="s">
+        <v>332</v>
+      </c>
+      <c r="H38" s="73" t="s">
+        <v>333</v>
+      </c>
+      <c r="I38" s="42">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="A39" s="42">
+        <v>3</v>
+      </c>
+      <c r="B39" s="42">
+        <v>38</v>
+      </c>
+      <c r="C39" s="42">
+        <v>0</v>
+      </c>
+      <c r="D39" s="43">
+        <v>1</v>
+      </c>
+      <c r="E39" s="42">
+        <v>2</v>
+      </c>
+      <c r="F39" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G39" s="73" t="s">
+        <v>332</v>
+      </c>
+      <c r="H39" s="73" t="s">
+        <v>333</v>
+      </c>
+      <c r="I39" s="42">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="A40" s="42">
+        <v>3</v>
+      </c>
+      <c r="B40" s="42">
+        <v>39</v>
+      </c>
+      <c r="C40" s="42">
+        <v>1</v>
+      </c>
+      <c r="D40" s="43">
+        <v>2</v>
+      </c>
+      <c r="E40" s="42">
+        <v>1</v>
+      </c>
+      <c r="F40" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G40" s="45" t="s">
+        <v>335</v>
+      </c>
+      <c r="H40" s="73" t="s">
+        <v>334</v>
+      </c>
+      <c r="I40" s="42">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="A41" s="42">
+        <v>3</v>
+      </c>
+      <c r="B41" s="42">
+        <v>40</v>
+      </c>
+      <c r="C41" s="42">
+        <v>1</v>
+      </c>
+      <c r="D41" s="43">
+        <v>2</v>
+      </c>
+      <c r="E41" s="42">
+        <v>1</v>
+      </c>
+      <c r="F41" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G41" s="45" t="s">
+        <v>335</v>
+      </c>
+      <c r="H41" s="73" t="s">
+        <v>334</v>
+      </c>
+      <c r="I41" s="42">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="A42" s="42">
+        <v>3</v>
+      </c>
+      <c r="B42" s="42">
+        <v>41</v>
+      </c>
+      <c r="C42" s="42">
+        <v>0</v>
+      </c>
+      <c r="D42" s="43">
+        <v>2</v>
+      </c>
+      <c r="E42" s="42">
+        <v>1</v>
+      </c>
+      <c r="F42" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G42" s="74" t="s">
+        <v>336</v>
+      </c>
+      <c r="H42" s="73" t="s">
+        <v>334</v>
+      </c>
+      <c r="I42" s="42"/>
+    </row>
+    <row r="43" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="A43" s="42">
+        <v>3</v>
+      </c>
+      <c r="B43" s="42">
+        <v>42</v>
+      </c>
+      <c r="C43" s="42">
+        <v>1</v>
+      </c>
+      <c r="D43" s="43">
+        <v>2</v>
+      </c>
+      <c r="E43" s="42">
+        <v>2</v>
+      </c>
+      <c r="F43" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G43" s="74" t="s">
+        <v>336</v>
+      </c>
+      <c r="H43" s="73" t="s">
+        <v>334</v>
+      </c>
+      <c r="I43" s="42"/>
+    </row>
+    <row r="44" spans="1:9" s="13" customFormat="1">
+      <c r="A44" s="9">
+        <v>1</v>
+      </c>
+      <c r="B44" s="9">
+        <v>43</v>
+      </c>
+      <c r="C44" s="9">
+        <v>0</v>
+      </c>
+      <c r="D44" s="10">
+        <v>1</v>
+      </c>
+      <c r="E44" s="9">
+        <v>1</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="G44" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="H23" s="11" t="s">
+      <c r="H44" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" s="13" customFormat="1">
-      <c r="A24" s="9">
-        <v>1</v>
-      </c>
-      <c r="B24" s="9">
+      <c r="I44" s="9"/>
+    </row>
+    <row r="45" spans="1:9" s="13" customFormat="1">
+      <c r="A45" s="9">
+        <v>1</v>
+      </c>
+      <c r="B45" s="9">
         <v>44</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C45" s="9">
         <v>0</v>
       </c>
-      <c r="D24" s="10">
-        <v>1</v>
-      </c>
-      <c r="E24" s="9">
-        <v>1</v>
-      </c>
-      <c r="F24" s="10" t="s">
+      <c r="D45" s="10">
+        <v>1</v>
+      </c>
+      <c r="E45" s="9">
+        <v>1</v>
+      </c>
+      <c r="F45" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G45" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="H45" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" s="13" customFormat="1" ht="30">
-      <c r="A25" s="9">
-        <v>1</v>
-      </c>
-      <c r="B25" s="9">
+      <c r="I45" s="9"/>
+    </row>
+    <row r="46" spans="1:9" s="13" customFormat="1" ht="30">
+      <c r="A46" s="9">
+        <v>1</v>
+      </c>
+      <c r="B46" s="9">
         <v>45</v>
       </c>
-      <c r="C25" s="9">
-        <v>1</v>
-      </c>
-      <c r="D25" s="10">
-        <v>1</v>
-      </c>
-      <c r="E25" s="9">
-        <v>2</v>
-      </c>
-      <c r="F25" s="10" t="s">
+      <c r="C46" s="9">
+        <v>1</v>
+      </c>
+      <c r="D46" s="10">
+        <v>1</v>
+      </c>
+      <c r="E46" s="9">
+        <v>2</v>
+      </c>
+      <c r="F46" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G46" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="H25" s="12" t="s">
+      <c r="H46" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" s="13" customFormat="1" ht="30">
-      <c r="A26" s="9">
-        <v>1</v>
-      </c>
-      <c r="B26" s="9">
+      <c r="I46" s="9"/>
+    </row>
+    <row r="47" spans="1:9" s="13" customFormat="1" ht="30">
+      <c r="A47" s="9">
+        <v>1</v>
+      </c>
+      <c r="B47" s="9">
         <v>46</v>
       </c>
-      <c r="C26" s="9">
-        <v>1</v>
-      </c>
-      <c r="D26" s="10">
-        <v>1</v>
-      </c>
-      <c r="E26" s="9">
-        <v>1</v>
-      </c>
-      <c r="F26" s="10" t="s">
+      <c r="C47" s="9">
+        <v>1</v>
+      </c>
+      <c r="D47" s="10">
+        <v>1</v>
+      </c>
+      <c r="E47" s="9">
+        <v>1</v>
+      </c>
+      <c r="F47" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G47" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="H26" s="12" t="s">
+      <c r="H47" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="1:9" s="13" customFormat="1">
-      <c r="A27" s="9">
-        <v>1</v>
-      </c>
-      <c r="B27" s="9">
+      <c r="I47" s="9"/>
+    </row>
+    <row r="48" spans="1:9" s="13" customFormat="1">
+      <c r="A48" s="9">
+        <v>1</v>
+      </c>
+      <c r="B48" s="9">
         <v>47</v>
       </c>
-      <c r="C27" s="9">
-        <v>1</v>
-      </c>
-      <c r="D27" s="10">
-        <v>2</v>
-      </c>
-      <c r="E27" s="9">
-        <v>1</v>
-      </c>
-      <c r="F27" s="10" t="s">
+      <c r="C48" s="9">
+        <v>1</v>
+      </c>
+      <c r="D48" s="10">
+        <v>2</v>
+      </c>
+      <c r="E48" s="9">
+        <v>1</v>
+      </c>
+      <c r="F48" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G48" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H48" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="I27" s="9"/>
-    </row>
-    <row r="28" spans="1:9" s="46" customFormat="1">
-      <c r="A28" s="42">
-        <v>3</v>
-      </c>
-      <c r="B28" s="42">
+      <c r="I48" s="9"/>
+    </row>
+    <row r="49" spans="1:9" s="46" customFormat="1">
+      <c r="A49" s="42">
+        <v>3</v>
+      </c>
+      <c r="B49" s="42">
+        <v>48</v>
+      </c>
+      <c r="C49" s="42">
+        <v>1</v>
+      </c>
+      <c r="D49" s="43">
+        <v>2</v>
+      </c>
+      <c r="E49" s="42">
+        <v>1</v>
+      </c>
+      <c r="F49" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G49" s="44" t="s">
+        <v>189</v>
+      </c>
+      <c r="H49" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="I49" s="42" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="46" customFormat="1">
+      <c r="A50" s="42">
+        <v>3</v>
+      </c>
+      <c r="B50" s="42">
+        <v>49</v>
+      </c>
+      <c r="C50" s="42">
+        <v>1</v>
+      </c>
+      <c r="D50" s="43">
+        <v>2</v>
+      </c>
+      <c r="E50" s="42">
+        <v>1</v>
+      </c>
+      <c r="F50" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G50" s="44" t="s">
+        <v>189</v>
+      </c>
+      <c r="H50" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="I50" s="42">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="46" customFormat="1">
+      <c r="A51" s="42">
+        <v>3</v>
+      </c>
+      <c r="B51" s="42">
+        <v>50</v>
+      </c>
+      <c r="C51" s="42">
+        <v>1</v>
+      </c>
+      <c r="D51" s="43">
+        <v>2</v>
+      </c>
+      <c r="E51" s="42">
+        <v>2</v>
+      </c>
+      <c r="F51" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G51" s="44" t="s">
+        <v>189</v>
+      </c>
+      <c r="H51" s="44" t="s">
+        <v>338</v>
+      </c>
+      <c r="I51" s="42"/>
+    </row>
+    <row r="52" spans="1:9" s="46" customFormat="1">
+      <c r="A52" s="42">
+        <v>3</v>
+      </c>
+      <c r="B52" s="42">
+        <v>51</v>
+      </c>
+      <c r="C52" s="42">
+        <v>1</v>
+      </c>
+      <c r="D52" s="43">
+        <v>2</v>
+      </c>
+      <c r="E52" s="42">
+        <v>3</v>
+      </c>
+      <c r="F52" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G52" s="44" t="s">
+        <v>189</v>
+      </c>
+      <c r="H52" s="44" t="s">
+        <v>338</v>
+      </c>
+      <c r="I52" s="42"/>
+    </row>
+    <row r="53" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="A53" s="42">
+        <v>3</v>
+      </c>
+      <c r="B53" s="42">
+        <v>52</v>
+      </c>
+      <c r="C53" s="42">
+        <v>1</v>
+      </c>
+      <c r="D53" s="43">
+        <v>2</v>
+      </c>
+      <c r="E53" s="42">
+        <v>1</v>
+      </c>
+      <c r="F53" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G53" s="74" t="s">
+        <v>339</v>
+      </c>
+      <c r="H53" s="73" t="s">
+        <v>340</v>
+      </c>
+      <c r="I53" s="42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="A54" s="42">
+        <v>3</v>
+      </c>
+      <c r="B54" s="42">
+        <v>53</v>
+      </c>
+      <c r="C54" s="42">
+        <v>1</v>
+      </c>
+      <c r="D54" s="43">
+        <v>2</v>
+      </c>
+      <c r="E54" s="42">
+        <v>2</v>
+      </c>
+      <c r="F54" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G54" s="74" t="s">
+        <v>339</v>
+      </c>
+      <c r="H54" s="73" t="s">
+        <v>340</v>
+      </c>
+      <c r="I54" s="42">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="A55" s="42">
+        <v>3</v>
+      </c>
+      <c r="B55" s="42">
+        <v>54</v>
+      </c>
+      <c r="C55" s="42">
+        <v>1</v>
+      </c>
+      <c r="D55" s="43">
+        <v>2</v>
+      </c>
+      <c r="E55" s="42">
+        <v>2</v>
+      </c>
+      <c r="F55" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G55" s="44" t="s">
+        <v>189</v>
+      </c>
+      <c r="H55" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="I55" s="42"/>
+    </row>
+    <row r="56" spans="1:9" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="A56" s="42">
+        <v>3</v>
+      </c>
+      <c r="B56" s="42">
+        <v>55</v>
+      </c>
+      <c r="C56" s="42">
+        <v>1</v>
+      </c>
+      <c r="D56" s="43">
+        <v>1</v>
+      </c>
+      <c r="E56" s="42">
+        <v>2</v>
+      </c>
+      <c r="F56" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G56" s="44" t="s">
+        <v>189</v>
+      </c>
+      <c r="H56" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="I56" s="42"/>
+    </row>
+    <row r="57" spans="1:9" s="46" customFormat="1">
+      <c r="A57" s="42">
+        <v>3</v>
+      </c>
+      <c r="B57" s="42">
         <v>61</v>
       </c>
-      <c r="C28" s="42">
-        <v>1</v>
-      </c>
-      <c r="D28" s="43">
-        <v>2</v>
-      </c>
-      <c r="E28" s="42">
-        <v>1</v>
-      </c>
-      <c r="F28" s="43" t="s">
+      <c r="C57" s="42">
+        <v>1</v>
+      </c>
+      <c r="D57" s="43">
+        <v>2</v>
+      </c>
+      <c r="E57" s="42">
+        <v>1</v>
+      </c>
+      <c r="F57" s="43" t="s">
         <v>249</v>
       </c>
-      <c r="G28" s="44" t="s">
+      <c r="G57" s="44" t="s">
         <v>189</v>
       </c>
-      <c r="H28" s="44" t="s">
+      <c r="H57" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="I28" s="42">
+      <c r="I57" s="42">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="46" customFormat="1">
-      <c r="A29" s="42">
-        <v>3</v>
-      </c>
-      <c r="B29" s="42">
+    <row r="58" spans="1:9" s="46" customFormat="1">
+      <c r="A58" s="42">
+        <v>3</v>
+      </c>
+      <c r="B58" s="42">
         <v>62</v>
       </c>
-      <c r="C29" s="42">
-        <v>1</v>
-      </c>
-      <c r="D29" s="43">
-        <v>2</v>
-      </c>
-      <c r="E29" s="42">
-        <v>3</v>
-      </c>
-      <c r="F29" s="43" t="s">
+      <c r="C58" s="42">
+        <v>1</v>
+      </c>
+      <c r="D58" s="43">
+        <v>2</v>
+      </c>
+      <c r="E58" s="42">
+        <v>3</v>
+      </c>
+      <c r="F58" s="43" t="s">
         <v>249</v>
       </c>
-      <c r="G29" s="44" t="s">
+      <c r="G58" s="44" t="s">
         <v>189</v>
       </c>
-      <c r="H29" s="44" t="s">
+      <c r="H58" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="I29" s="42">
+      <c r="I58" s="42">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="13" customFormat="1">
-      <c r="A30" s="9">
-        <v>1</v>
-      </c>
-      <c r="B30" s="9">
+    <row r="59" spans="1:9" s="13" customFormat="1">
+      <c r="A59" s="9">
+        <v>1</v>
+      </c>
+      <c r="B59" s="9">
         <v>77</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C59" s="9">
         <v>0</v>
       </c>
-      <c r="D30" s="10">
-        <v>1</v>
-      </c>
-      <c r="E30" s="9">
-        <v>2</v>
-      </c>
-      <c r="F30" s="10" t="s">
+      <c r="D59" s="10">
+        <v>1</v>
+      </c>
+      <c r="E59" s="9">
+        <v>2</v>
+      </c>
+      <c r="F59" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="G59" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="H30" s="11" t="s">
+      <c r="H59" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="I30" s="9"/>
+      <c r="I59" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4523,8 +5391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J220"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B233" sqref="B233"/>
     </sheetView>
   </sheetViews>
@@ -11305,7 +12173,7 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
@@ -12751,9 +13619,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J77" sqref="J77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12934,7 +13802,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="50">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" s="54" t="s">
         <v>55</v>
@@ -13060,7 +13928,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="54" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Updated lists and questions
</commit_message>
<xml_diff>
--- a/lists/lists.rs.xlsx
+++ b/lists/lists.rs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="2895" windowWidth="15600" windowHeight="5190" activeTab="4"/>
+    <workbookView xWindow="210" yWindow="2895" windowWidth="15600" windowHeight="5190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="fractions" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1965" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="358">
   <si>
     <t>RAZRED</t>
   </si>
@@ -1138,6 +1138,18 @@
   </si>
   <si>
     <t>Simetrične figure</t>
+  </si>
+  <si>
+    <t>Podaci</t>
+  </si>
+  <si>
+    <t>Tabela i stubičasti dijagram</t>
+  </si>
+  <si>
+    <t>geom. 57</t>
+  </si>
+  <si>
+    <t>kockica za igru</t>
   </si>
 </sst>
 </file>
@@ -1485,10 +1497,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFCC"/>
       <color rgb="FFFFCCCC"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FFCCECFF"/>
-      <color rgb="FFFFFFCC"/>
       <color rgb="FFCCFFFF"/>
       <color rgb="FF99FFCC"/>
       <color rgb="FF99CCFF"/>
@@ -3828,11 +3840,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J77" sqref="J77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H75" sqref="H74:H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6112,6 +6124,38 @@
       <c r="I78" s="11"/>
       <c r="J78" s="9"/>
     </row>
+    <row r="79" spans="1:10" s="53" customFormat="1" ht="15" customHeight="1">
+      <c r="A79" s="50">
+        <v>4</v>
+      </c>
+      <c r="B79" s="50">
+        <v>78</v>
+      </c>
+      <c r="C79" s="50">
+        <v>1</v>
+      </c>
+      <c r="D79" s="51">
+        <v>2</v>
+      </c>
+      <c r="E79" s="50">
+        <v>2</v>
+      </c>
+      <c r="F79" s="51" t="s">
+        <v>248</v>
+      </c>
+      <c r="G79" s="56" t="s">
+        <v>328</v>
+      </c>
+      <c r="H79" s="56" t="s">
+        <v>326</v>
+      </c>
+      <c r="I79" s="56" t="s">
+        <v>357</v>
+      </c>
+      <c r="J79" s="50">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6120,11 +6164,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J220"/>
+  <dimension ref="A1:J224"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G237" sqref="G237"/>
+      <pane ySplit="1" topLeftCell="A220" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J224" sqref="J224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11118,33 +11162,35 @@
       </c>
       <c r="J162" s="19"/>
     </row>
-    <row r="163" spans="1:10" s="22" customFormat="1">
-      <c r="A163" s="36" t="s">
+    <row r="163" spans="1:10" s="46" customFormat="1">
+      <c r="A163" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="B163" s="19">
+      <c r="B163" s="42">
         <v>162</v>
       </c>
-      <c r="C163" s="19">
-        <v>1</v>
-      </c>
-      <c r="D163" s="20">
-        <v>1</v>
-      </c>
-      <c r="E163" s="19"/>
-      <c r="F163" s="20" t="s">
-        <v>247</v>
-      </c>
-      <c r="G163" s="21" t="s">
+      <c r="C163" s="42">
+        <v>1</v>
+      </c>
+      <c r="D163" s="43">
+        <v>1</v>
+      </c>
+      <c r="E163" s="42">
+        <v>2</v>
+      </c>
+      <c r="F163" s="43" t="s">
+        <v>247</v>
+      </c>
+      <c r="G163" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="H163" s="23" t="s">
+      <c r="H163" s="45" t="s">
         <v>122</v>
       </c>
-      <c r="I163" s="23" t="s">
+      <c r="I163" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="J163" s="19"/>
+      <c r="J163" s="42"/>
     </row>
     <row r="164" spans="1:10" s="22" customFormat="1">
       <c r="A164" s="36" t="s">
@@ -12888,6 +12934,128 @@
       </c>
       <c r="J220" s="50">
         <v>105</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" s="22" customFormat="1">
+      <c r="A221" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B221" s="19">
+        <v>220</v>
+      </c>
+      <c r="C221" s="19">
+        <v>1</v>
+      </c>
+      <c r="D221" s="20">
+        <v>3</v>
+      </c>
+      <c r="E221" s="19">
+        <v>1</v>
+      </c>
+      <c r="F221" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="G221" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="H221" s="21" t="s">
+        <v>355</v>
+      </c>
+      <c r="I221" s="23"/>
+      <c r="J221" s="19"/>
+    </row>
+    <row r="222" spans="1:10" s="22" customFormat="1">
+      <c r="A222" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B222" s="19">
+        <v>221</v>
+      </c>
+      <c r="C222" s="19">
+        <v>1</v>
+      </c>
+      <c r="D222" s="20">
+        <v>1</v>
+      </c>
+      <c r="E222" s="19">
+        <v>2</v>
+      </c>
+      <c r="F222" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="G222" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="H222" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="I222" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="J222" s="19" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" s="13" customFormat="1" ht="30">
+      <c r="A223" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B223" s="9">
+        <v>222</v>
+      </c>
+      <c r="C223" s="9">
+        <v>1</v>
+      </c>
+      <c r="D223" s="10">
+        <v>3</v>
+      </c>
+      <c r="E223" s="9">
+        <v>2</v>
+      </c>
+      <c r="F223" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="G223" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H223" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I223" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="J223" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" s="22" customFormat="1">
+      <c r="A224" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B224" s="19">
+        <v>223</v>
+      </c>
+      <c r="C224" s="19">
+        <v>1</v>
+      </c>
+      <c r="D224" s="20">
+        <v>3</v>
+      </c>
+      <c r="E224" s="19">
+        <v>1</v>
+      </c>
+      <c r="F224" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="G224" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="H224" s="21" t="s">
+        <v>355</v>
+      </c>
+      <c r="I224" s="23"/>
+      <c r="J224" s="19">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -14348,11 +14516,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15695,42 +15863,44 @@
       </c>
       <c r="J44" s="57"/>
     </row>
-    <row r="45" spans="1:10" s="60" customFormat="1">
-      <c r="A45" s="57">
-        <v>2</v>
-      </c>
-      <c r="B45" s="57">
-        <v>48</v>
-      </c>
-      <c r="C45" s="57">
-        <v>1</v>
-      </c>
-      <c r="D45" s="58">
-        <v>1</v>
-      </c>
-      <c r="E45" s="57">
-        <v>1</v>
-      </c>
-      <c r="F45" s="61" t="s">
+    <row r="45" spans="1:10" s="46" customFormat="1">
+      <c r="A45" s="42">
+        <v>3</v>
+      </c>
+      <c r="B45" s="42">
+        <v>44</v>
+      </c>
+      <c r="C45" s="42">
+        <v>1</v>
+      </c>
+      <c r="D45" s="43">
+        <v>2</v>
+      </c>
+      <c r="E45" s="42">
+        <v>2</v>
+      </c>
+      <c r="F45" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="G45" s="59" t="s">
+      <c r="G45" s="44" t="s">
         <v>252</v>
       </c>
-      <c r="H45" s="61" t="s">
-        <v>251</v>
-      </c>
-      <c r="I45" s="70" t="s">
-        <v>260</v>
-      </c>
-      <c r="J45" s="57"/>
+      <c r="H45" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="I45" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="J45" s="42">
+        <v>51</v>
+      </c>
     </row>
     <row r="46" spans="1:10" s="60" customFormat="1">
       <c r="A46" s="57">
         <v>2</v>
       </c>
       <c r="B46" s="57">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C46" s="57">
         <v>1</v>
@@ -15739,7 +15909,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" s="61" t="s">
         <v>54</v>
@@ -15747,11 +15917,11 @@
       <c r="G46" s="59" t="s">
         <v>252</v>
       </c>
-      <c r="H46" s="59" t="s">
-        <v>171</v>
-      </c>
-      <c r="I46" s="69" t="s">
-        <v>37</v>
+      <c r="H46" s="61" t="s">
+        <v>251</v>
+      </c>
+      <c r="I46" s="70" t="s">
+        <v>260</v>
       </c>
       <c r="J46" s="57"/>
     </row>
@@ -15760,7 +15930,7 @@
         <v>2</v>
       </c>
       <c r="B47" s="57">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C47" s="57">
         <v>1</v>
@@ -15790,7 +15960,7 @@
         <v>2</v>
       </c>
       <c r="B48" s="57">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C48" s="57">
         <v>1</v>
@@ -15799,7 +15969,7 @@
         <v>1</v>
       </c>
       <c r="E48" s="57">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" s="61" t="s">
         <v>54</v>
@@ -15815,45 +15985,43 @@
       </c>
       <c r="J48" s="57"/>
     </row>
-    <row r="49" spans="1:10" s="46" customFormat="1">
-      <c r="A49" s="42">
-        <v>3</v>
-      </c>
-      <c r="B49" s="42">
+    <row r="49" spans="1:10" s="60" customFormat="1">
+      <c r="A49" s="57">
+        <v>2</v>
+      </c>
+      <c r="B49" s="57">
+        <v>51</v>
+      </c>
+      <c r="C49" s="57">
+        <v>1</v>
+      </c>
+      <c r="D49" s="58">
+        <v>1</v>
+      </c>
+      <c r="E49" s="57">
+        <v>3</v>
+      </c>
+      <c r="F49" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="G49" s="59" t="s">
+        <v>252</v>
+      </c>
+      <c r="H49" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="I49" s="69" t="s">
+        <v>37</v>
+      </c>
+      <c r="J49" s="57"/>
+    </row>
+    <row r="50" spans="1:10" s="46" customFormat="1">
+      <c r="A50" s="42">
+        <v>3</v>
+      </c>
+      <c r="B50" s="42">
         <v>52</v>
       </c>
-      <c r="C49" s="42">
-        <v>1</v>
-      </c>
-      <c r="D49" s="43">
-        <v>2</v>
-      </c>
-      <c r="E49" s="42">
-        <v>2</v>
-      </c>
-      <c r="F49" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="G49" s="44" t="s">
-        <v>252</v>
-      </c>
-      <c r="H49" s="44" t="s">
-        <v>171</v>
-      </c>
-      <c r="I49" s="67" t="s">
-        <v>37</v>
-      </c>
-      <c r="J49" s="42">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" s="46" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A50" s="42">
-        <v>3</v>
-      </c>
-      <c r="B50" s="42">
-        <v>53</v>
-      </c>
       <c r="C50" s="42">
         <v>1</v>
       </c>
@@ -15861,7 +16029,7 @@
         <v>2</v>
       </c>
       <c r="E50" s="42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F50" s="45" t="s">
         <v>54</v>
@@ -15869,20 +16037,22 @@
       <c r="G50" s="44" t="s">
         <v>252</v>
       </c>
-      <c r="H50" s="45" t="s">
-        <v>251</v>
+      <c r="H50" s="44" t="s">
+        <v>171</v>
       </c>
       <c r="I50" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="J50" s="42"/>
-    </row>
-    <row r="51" spans="1:10" s="46" customFormat="1">
+      <c r="J50" s="42">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="46" customFormat="1" ht="17.25" customHeight="1">
       <c r="A51" s="42">
         <v>3</v>
       </c>
       <c r="B51" s="42">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C51" s="42">
         <v>1</v>
@@ -15891,19 +16061,19 @@
         <v>2</v>
       </c>
       <c r="E51" s="42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" s="45" t="s">
         <v>54</v>
       </c>
       <c r="G51" s="44" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="H51" s="45" t="s">
         <v>251</v>
       </c>
-      <c r="I51" s="71" t="s">
-        <v>256</v>
+      <c r="I51" s="67" t="s">
+        <v>37</v>
       </c>
       <c r="J51" s="42"/>
     </row>
@@ -15912,7 +16082,7 @@
         <v>3</v>
       </c>
       <c r="B52" s="42">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C52" s="42">
         <v>1</v>
@@ -15921,7 +16091,7 @@
         <v>2</v>
       </c>
       <c r="E52" s="42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F52" s="45" t="s">
         <v>54</v>
@@ -15942,7 +16112,7 @@
         <v>3</v>
       </c>
       <c r="B53" s="42">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C53" s="42">
         <v>1</v>
@@ -15951,7 +16121,7 @@
         <v>2</v>
       </c>
       <c r="E53" s="42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" s="45" t="s">
         <v>54</v>
@@ -15972,7 +16142,7 @@
         <v>3</v>
       </c>
       <c r="B54" s="42">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C54" s="42">
         <v>1</v>
@@ -15987,13 +16157,13 @@
         <v>54</v>
       </c>
       <c r="G54" s="44" t="s">
-        <v>252</v>
-      </c>
-      <c r="H54" s="44" t="s">
-        <v>171</v>
-      </c>
-      <c r="I54" s="67" t="s">
-        <v>267</v>
+        <v>249</v>
+      </c>
+      <c r="H54" s="45" t="s">
+        <v>251</v>
+      </c>
+      <c r="I54" s="71" t="s">
+        <v>256</v>
       </c>
       <c r="J54" s="42"/>
     </row>
@@ -16002,7 +16172,7 @@
         <v>3</v>
       </c>
       <c r="B55" s="42">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C55" s="42">
         <v>1</v>
@@ -16017,24 +16187,22 @@
         <v>54</v>
       </c>
       <c r="G55" s="44" t="s">
-        <v>249</v>
-      </c>
-      <c r="H55" s="45" t="s">
-        <v>251</v>
-      </c>
-      <c r="I55" s="71" t="s">
-        <v>256</v>
-      </c>
-      <c r="J55" s="42">
-        <v>56</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="H55" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="I55" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="J55" s="42"/>
     </row>
     <row r="56" spans="1:10" s="46" customFormat="1">
       <c r="A56" s="42">
         <v>3</v>
       </c>
       <c r="B56" s="42">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C56" s="42">
         <v>1</v>
@@ -16051,14 +16219,14 @@
       <c r="G56" s="44" t="s">
         <v>249</v>
       </c>
-      <c r="H56" s="44" t="s">
-        <v>266</v>
+      <c r="H56" s="45" t="s">
+        <v>251</v>
       </c>
       <c r="I56" s="71" t="s">
         <v>256</v>
       </c>
       <c r="J56" s="42">
-        <v>30</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="46" customFormat="1">
@@ -16066,7 +16234,7 @@
         <v>3</v>
       </c>
       <c r="B57" s="42">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C57" s="42">
         <v>1</v>
@@ -16084,13 +16252,13 @@
         <v>249</v>
       </c>
       <c r="H57" s="44" t="s">
-        <v>171</v>
+        <v>266</v>
       </c>
       <c r="I57" s="71" t="s">
         <v>256</v>
       </c>
       <c r="J57" s="42">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="46" customFormat="1">
@@ -16098,7 +16266,7 @@
         <v>3</v>
       </c>
       <c r="B58" s="42">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C58" s="42">
         <v>1</v>
@@ -16107,28 +16275,30 @@
         <v>2</v>
       </c>
       <c r="E58" s="42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F58" s="45" t="s">
         <v>54</v>
       </c>
       <c r="G58" s="44" t="s">
-        <v>261</v>
-      </c>
-      <c r="H58" s="45" t="s">
-        <v>251</v>
+        <v>249</v>
+      </c>
+      <c r="H58" s="44" t="s">
+        <v>171</v>
       </c>
       <c r="I58" s="71" t="s">
-        <v>268</v>
-      </c>
-      <c r="J58" s="42"/>
+        <v>256</v>
+      </c>
+      <c r="J58" s="42">
+        <v>31</v>
+      </c>
     </row>
     <row r="59" spans="1:10" s="46" customFormat="1">
       <c r="A59" s="42">
         <v>3</v>
       </c>
       <c r="B59" s="42">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C59" s="42">
         <v>1</v>
@@ -16149,7 +16319,7 @@
         <v>251</v>
       </c>
       <c r="I59" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J59" s="42"/>
     </row>
@@ -16158,7 +16328,7 @@
         <v>3</v>
       </c>
       <c r="B60" s="42">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C60" s="42">
         <v>1</v>
@@ -16167,7 +16337,7 @@
         <v>2</v>
       </c>
       <c r="E60" s="42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" s="45" t="s">
         <v>54</v>
@@ -16183,12 +16353,12 @@
       </c>
       <c r="J60" s="42"/>
     </row>
-    <row r="61" spans="1:10" s="46" customFormat="1" ht="19.5" customHeight="1">
+    <row r="61" spans="1:10" s="46" customFormat="1">
       <c r="A61" s="42">
         <v>3</v>
       </c>
       <c r="B61" s="42">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C61" s="42">
         <v>1</v>
@@ -16205,7 +16375,7 @@
       <c r="G61" s="44" t="s">
         <v>261</v>
       </c>
-      <c r="H61" s="44" t="s">
+      <c r="H61" s="45" t="s">
         <v>251</v>
       </c>
       <c r="I61" s="71" t="s">
@@ -16213,12 +16383,12 @@
       </c>
       <c r="J61" s="42"/>
     </row>
-    <row r="62" spans="1:10" s="46" customFormat="1">
+    <row r="62" spans="1:10" s="46" customFormat="1" ht="19.5" customHeight="1">
       <c r="A62" s="42">
         <v>3</v>
       </c>
       <c r="B62" s="42">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C62" s="42">
         <v>1</v>
@@ -16236,7 +16406,7 @@
         <v>261</v>
       </c>
       <c r="H62" s="44" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="I62" s="71" t="s">
         <v>269</v>
@@ -16248,7 +16418,7 @@
         <v>3</v>
       </c>
       <c r="B63" s="42">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C63" s="42">
         <v>1</v>
@@ -16266,7 +16436,7 @@
         <v>261</v>
       </c>
       <c r="H63" s="44" t="s">
-        <v>171</v>
+        <v>266</v>
       </c>
       <c r="I63" s="71" t="s">
         <v>269</v>
@@ -16278,7 +16448,7 @@
         <v>3</v>
       </c>
       <c r="B64" s="42">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C64" s="42">
         <v>1</v>
@@ -16287,28 +16457,28 @@
         <v>2</v>
       </c>
       <c r="E64" s="42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F64" s="45" t="s">
         <v>54</v>
       </c>
       <c r="G64" s="44" t="s">
-        <v>262</v>
-      </c>
-      <c r="H64" s="45" t="s">
-        <v>251</v>
+        <v>261</v>
+      </c>
+      <c r="H64" s="44" t="s">
+        <v>171</v>
       </c>
       <c r="I64" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J64" s="42"/>
     </row>
-    <row r="65" spans="1:10" s="46" customFormat="1" ht="28.5" customHeight="1">
+    <row r="65" spans="1:10" s="46" customFormat="1">
       <c r="A65" s="42">
         <v>3</v>
       </c>
       <c r="B65" s="42">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C65" s="42">
         <v>1</v>
@@ -16322,23 +16492,23 @@
       <c r="F65" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="G65" s="45" t="s">
-        <v>263</v>
-      </c>
-      <c r="H65" s="44" t="s">
-        <v>264</v>
+      <c r="G65" s="44" t="s">
+        <v>262</v>
+      </c>
+      <c r="H65" s="45" t="s">
+        <v>251</v>
       </c>
       <c r="I65" s="71" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J65" s="42"/>
     </row>
-    <row r="66" spans="1:10" s="46" customFormat="1" ht="30">
+    <row r="66" spans="1:10" s="46" customFormat="1" ht="28.5" customHeight="1">
       <c r="A66" s="42">
         <v>3</v>
       </c>
       <c r="B66" s="42">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C66" s="42">
         <v>1</v>
@@ -16355,7 +16525,7 @@
       <c r="G66" s="45" t="s">
         <v>263</v>
       </c>
-      <c r="H66" s="45" t="s">
+      <c r="H66" s="44" t="s">
         <v>264</v>
       </c>
       <c r="I66" s="71" t="s">
@@ -16363,12 +16533,12 @@
       </c>
       <c r="J66" s="42"/>
     </row>
-    <row r="67" spans="1:10" s="46" customFormat="1">
+    <row r="67" spans="1:10" s="46" customFormat="1" ht="30">
       <c r="A67" s="42">
         <v>3</v>
       </c>
       <c r="B67" s="42">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C67" s="42">
         <v>1</v>
@@ -16382,14 +16552,14 @@
       <c r="F67" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="G67" s="44" t="s">
-        <v>262</v>
-      </c>
-      <c r="H67" s="46" t="s">
-        <v>171</v>
-      </c>
-      <c r="I67" s="44" t="s">
-        <v>37</v>
+      <c r="G67" s="45" t="s">
+        <v>263</v>
+      </c>
+      <c r="H67" s="45" t="s">
+        <v>264</v>
+      </c>
+      <c r="I67" s="71" t="s">
+        <v>271</v>
       </c>
       <c r="J67" s="42"/>
     </row>
@@ -16398,7 +16568,7 @@
         <v>3</v>
       </c>
       <c r="B68" s="42">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C68" s="42">
         <v>1</v>
@@ -16413,7 +16583,7 @@
         <v>54</v>
       </c>
       <c r="G68" s="44" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H68" s="46" t="s">
         <v>171</v>
@@ -16428,7 +16598,7 @@
         <v>3</v>
       </c>
       <c r="B69" s="42">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C69" s="42">
         <v>1</v>
@@ -16443,10 +16613,10 @@
         <v>54</v>
       </c>
       <c r="G69" s="44" t="s">
-        <v>252</v>
-      </c>
-      <c r="H69" s="44" t="s">
-        <v>266</v>
+        <v>261</v>
+      </c>
+      <c r="H69" s="46" t="s">
+        <v>171</v>
       </c>
       <c r="I69" s="44" t="s">
         <v>37</v>
@@ -16458,7 +16628,7 @@
         <v>3</v>
       </c>
       <c r="B70" s="42">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C70" s="42">
         <v>1</v>
@@ -16467,16 +16637,16 @@
         <v>2</v>
       </c>
       <c r="E70" s="42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" s="45" t="s">
         <v>54</v>
       </c>
       <c r="G70" s="44" t="s">
-        <v>261</v>
-      </c>
-      <c r="H70" s="46" t="s">
-        <v>171</v>
+        <v>252</v>
+      </c>
+      <c r="H70" s="44" t="s">
+        <v>266</v>
       </c>
       <c r="I70" s="44" t="s">
         <v>37</v>
@@ -16488,7 +16658,7 @@
         <v>3</v>
       </c>
       <c r="B71" s="42">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C71" s="42">
         <v>1</v>
@@ -16503,7 +16673,7 @@
         <v>54</v>
       </c>
       <c r="G71" s="44" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="H71" s="46" t="s">
         <v>171</v>
@@ -16513,44 +16683,42 @@
       </c>
       <c r="J71" s="42"/>
     </row>
-    <row r="72" spans="1:10" s="53" customFormat="1">
-      <c r="A72" s="50">
-        <v>4</v>
-      </c>
-      <c r="B72" s="50">
-        <v>77</v>
-      </c>
-      <c r="C72" s="50">
-        <v>1</v>
-      </c>
-      <c r="D72" s="51">
-        <v>1</v>
-      </c>
-      <c r="E72" s="50">
-        <v>2</v>
-      </c>
-      <c r="F72" s="54" t="s">
+    <row r="72" spans="1:10" s="46" customFormat="1">
+      <c r="A72" s="42">
+        <v>3</v>
+      </c>
+      <c r="B72" s="42">
+        <v>76</v>
+      </c>
+      <c r="C72" s="42">
+        <v>1</v>
+      </c>
+      <c r="D72" s="43">
+        <v>2</v>
+      </c>
+      <c r="E72" s="42">
+        <v>2</v>
+      </c>
+      <c r="F72" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="G72" s="52" t="s">
-        <v>321</v>
-      </c>
-      <c r="H72" s="52" t="s">
-        <v>322</v>
-      </c>
-      <c r="I72" s="52" t="s">
-        <v>314</v>
-      </c>
-      <c r="J72" s="50">
-        <v>4</v>
-      </c>
+      <c r="G72" s="44" t="s">
+        <v>252</v>
+      </c>
+      <c r="H72" s="46" t="s">
+        <v>171</v>
+      </c>
+      <c r="I72" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="J72" s="42"/>
     </row>
     <row r="73" spans="1:10" s="53" customFormat="1">
       <c r="A73" s="50">
         <v>4</v>
       </c>
       <c r="B73" s="50">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C73" s="50">
         <v>1</v>
@@ -16571,10 +16739,10 @@
         <v>322</v>
       </c>
       <c r="I73" s="52" t="s">
-        <v>299</v>
+        <v>314</v>
       </c>
       <c r="J73" s="50">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:10" s="53" customFormat="1">
@@ -16582,7 +16750,7 @@
         <v>4</v>
       </c>
       <c r="B74" s="50">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C74" s="50">
         <v>1</v>
@@ -16591,7 +16759,7 @@
         <v>1</v>
       </c>
       <c r="E74" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F74" s="54" t="s">
         <v>54</v>
@@ -16600,13 +16768,13 @@
         <v>321</v>
       </c>
       <c r="H74" s="52" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I74" s="52" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="J74" s="50">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:10" s="53" customFormat="1">
@@ -16614,7 +16782,7 @@
         <v>4</v>
       </c>
       <c r="B75" s="50">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C75" s="50">
         <v>1</v>
@@ -16623,7 +16791,7 @@
         <v>1</v>
       </c>
       <c r="E75" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" s="54" t="s">
         <v>54</v>
@@ -16634,11 +16802,11 @@
       <c r="H75" s="52" t="s">
         <v>323</v>
       </c>
-      <c r="I75" s="68" t="s">
-        <v>319</v>
+      <c r="I75" s="52" t="s">
+        <v>314</v>
       </c>
       <c r="J75" s="50">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:10" s="53" customFormat="1">
@@ -16646,7 +16814,7 @@
         <v>4</v>
       </c>
       <c r="B76" s="50">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C76" s="50">
         <v>1</v>
@@ -16655,7 +16823,7 @@
         <v>1</v>
       </c>
       <c r="E76" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F76" s="54" t="s">
         <v>54</v>
@@ -16666,11 +16834,11 @@
       <c r="H76" s="52" t="s">
         <v>323</v>
       </c>
-      <c r="I76" s="52" t="s">
-        <v>299</v>
+      <c r="I76" s="68" t="s">
+        <v>319</v>
       </c>
       <c r="J76" s="50">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:10" s="53" customFormat="1">
@@ -16678,7 +16846,7 @@
         <v>4</v>
       </c>
       <c r="B77" s="50">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C77" s="50">
         <v>1</v>
@@ -16687,7 +16855,7 @@
         <v>1</v>
       </c>
       <c r="E77" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" s="54" t="s">
         <v>54</v>
@@ -16702,7 +16870,7 @@
         <v>299</v>
       </c>
       <c r="J77" s="50">
-        <v>81</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:10" s="53" customFormat="1">
@@ -16710,7 +16878,7 @@
         <v>4</v>
       </c>
       <c r="B78" s="50">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C78" s="50">
         <v>1</v>
@@ -16734,6 +16902,38 @@
         <v>299</v>
       </c>
       <c r="J78" s="50">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" s="53" customFormat="1">
+      <c r="A79" s="50">
+        <v>4</v>
+      </c>
+      <c r="B79" s="50">
+        <v>83</v>
+      </c>
+      <c r="C79" s="50">
+        <v>1</v>
+      </c>
+      <c r="D79" s="51">
+        <v>1</v>
+      </c>
+      <c r="E79" s="50">
+        <v>2</v>
+      </c>
+      <c r="F79" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="G79" s="52" t="s">
+        <v>321</v>
+      </c>
+      <c r="H79" s="52" t="s">
+        <v>323</v>
+      </c>
+      <c r="I79" s="52" t="s">
+        <v>299</v>
+      </c>
+      <c r="J79" s="50">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new questions and lists. These now include years 5 and 6, but are not complete so are disabled by default. Added beta option to the URL to allow us to see the new years.
</commit_message>
<xml_diff>
--- a/lists/lists.rs.xlsx
+++ b/lists/lists.rs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="2895" windowWidth="15600" windowHeight="5190" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-90" windowWidth="15600" windowHeight="5190" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="fractions" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,18 @@
     <sheet name="numbers" sheetId="3" r:id="rId3"/>
     <sheet name="equations" sheetId="4" r:id="rId4"/>
     <sheet name="measures" sheetId="5" r:id="rId5"/>
+    <sheet name="fract_2" sheetId="6" r:id="rId6"/>
+    <sheet name="geom_2" sheetId="7" r:id="rId7"/>
+    <sheet name="numb_2" sheetId="8" r:id="rId8"/>
+    <sheet name="algebra" sheetId="9" r:id="rId9"/>
+    <sheet name="data" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2282" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2473" uniqueCount="358">
   <si>
     <t>RAZRED</t>
   </si>
@@ -1096,6 +1101,115 @@
   </si>
   <si>
     <t>dan, sedmica, mesec</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Dopuna niza članovima koji nedostaju</t>
+  </si>
+  <si>
+    <t>Tekstualni zadatak - temperatura</t>
+  </si>
+  <si>
+    <t>Poredjenje  brojeva</t>
+  </si>
+  <si>
+    <t>Razlika</t>
+  </si>
+  <si>
+    <t>Zajednički činioci dva broja</t>
+  </si>
+  <si>
+    <t>Deljivost sa 3, 6 i  9</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Celi brojevi</t>
+  </si>
+  <si>
+    <t>Prikaz na brojevnoj pravoj, upoređivanje</t>
+  </si>
+  <si>
+    <t>numbers 109</t>
+  </si>
+  <si>
+    <t>Pojam, suprotan broj, apsolutna vrednost</t>
+  </si>
+  <si>
+    <t>Zbir/razlika - tabela</t>
+  </si>
+  <si>
+    <t>Magični kvadrat</t>
+  </si>
+  <si>
+    <t>Deljivost brojeva</t>
+  </si>
+  <si>
+    <t>Svojstva deljivosti</t>
+  </si>
+  <si>
+    <t>Svi činioci  jednog broja</t>
+  </si>
+  <si>
+    <t>Deljivost sa 3 i 9</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">DEO                                   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Theme</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pojam, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">brojevna prava </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Proširivanje, skraćivanje i upoređivanje            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Računske operacije    </t>
+  </si>
+  <si>
+    <t>Mešoviti broj</t>
+  </si>
+  <si>
+    <t>Skraćivanje</t>
+  </si>
+  <si>
+    <t>Upoređivanje</t>
+  </si>
+  <si>
+    <t>Proširivanje</t>
+  </si>
+  <si>
+    <t>fract.20</t>
+  </si>
+  <si>
+    <t>fract.38</t>
   </si>
 </sst>
 </file>
@@ -1282,7 +1396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1509,6 +1623,21 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1517,10 +1646,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCCECFF"/>
       <color rgb="FFCCFFFF"/>
       <color rgb="FF99FFCC"/>
       <color rgb="FFFFFFCC"/>
-      <color rgb="FFCCECFF"/>
       <color rgb="FFFFCCCC"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FF99CCFF"/>
@@ -4178,13 +4307,78 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="36.75" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="I1" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="J1" s="76" t="s">
+        <v>326</v>
+      </c>
+      <c r="K1" s="58" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L93"/>
   <sheetViews>
     <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L93" sqref="L93"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7494,9 +7688,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M251"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K151" sqref="J151:K151"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A208" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16775,7 +16969,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18500,7 +18694,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G118" sqref="G118"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22600,4 +22794,1302 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="55" customFormat="1" ht="30">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="I1" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="J1" s="76" t="s">
+        <v>326</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" s="54" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="13" customFormat="1">
+      <c r="A2" s="9">
+        <v>5</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9">
+        <v>10</v>
+      </c>
+      <c r="D2" s="9">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9">
+        <v>1</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="95" t="s">
+        <v>349</v>
+      </c>
+      <c r="I2" s="10">
+        <v>4</v>
+      </c>
+      <c r="J2" s="10">
+        <v>1</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="13" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A3" s="9">
+        <v>5</v>
+      </c>
+      <c r="B3" s="9">
+        <v>2</v>
+      </c>
+      <c r="C3" s="9">
+        <v>10</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9">
+        <v>2</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="96" t="s">
+        <v>350</v>
+      </c>
+      <c r="I3" s="10">
+        <v>4</v>
+      </c>
+      <c r="J3" s="10">
+        <v>2</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="13" customFormat="1">
+      <c r="A4" s="9">
+        <v>5</v>
+      </c>
+      <c r="B4" s="9">
+        <v>3</v>
+      </c>
+      <c r="C4" s="9">
+        <v>10</v>
+      </c>
+      <c r="D4" s="9">
+        <v>2</v>
+      </c>
+      <c r="E4" s="9">
+        <v>2</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="I4" s="10">
+        <v>4</v>
+      </c>
+      <c r="J4" s="10">
+        <v>5</v>
+      </c>
+      <c r="K4" s="95" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="13" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A5" s="9">
+        <v>5</v>
+      </c>
+      <c r="B5" s="9">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9">
+        <v>8</v>
+      </c>
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="96" t="s">
+        <v>350</v>
+      </c>
+      <c r="I5" s="10">
+        <v>4</v>
+      </c>
+      <c r="J5" s="10">
+        <v>2</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="13" customFormat="1" ht="27" customHeight="1">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9">
+        <v>5</v>
+      </c>
+      <c r="C6" s="9">
+        <v>10</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9">
+        <v>1</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="96" t="s">
+        <v>350</v>
+      </c>
+      <c r="I6" s="10">
+        <v>4</v>
+      </c>
+      <c r="J6" s="10">
+        <v>2</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="13" customFormat="1" ht="27" customHeight="1">
+      <c r="A7" s="9">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9">
+        <v>6</v>
+      </c>
+      <c r="C7" s="9">
+        <v>10</v>
+      </c>
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9">
+        <v>2</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="96" t="s">
+        <v>350</v>
+      </c>
+      <c r="I7" s="10">
+        <v>4</v>
+      </c>
+      <c r="J7" s="10">
+        <v>2</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="13" customFormat="1" ht="27" customHeight="1">
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
+      <c r="B8" s="9">
+        <v>7</v>
+      </c>
+      <c r="C8" s="9">
+        <v>10</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="96" t="s">
+        <v>350</v>
+      </c>
+      <c r="I8" s="10">
+        <v>4</v>
+      </c>
+      <c r="J8" s="10">
+        <v>2</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="13" customFormat="1" ht="27" customHeight="1">
+      <c r="A9" s="9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="9">
+        <v>10</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="96" t="s">
+        <v>350</v>
+      </c>
+      <c r="I9" s="10">
+        <v>4</v>
+      </c>
+      <c r="J9" s="10">
+        <v>2</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="13" customFormat="1">
+      <c r="A10" s="9">
+        <v>5</v>
+      </c>
+      <c r="B10" s="9">
+        <v>9</v>
+      </c>
+      <c r="C10" s="9">
+        <v>10</v>
+      </c>
+      <c r="D10" s="9">
+        <v>2</v>
+      </c>
+      <c r="E10" s="9">
+        <v>2</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="I10" s="10">
+        <v>4</v>
+      </c>
+      <c r="J10" s="10">
+        <v>5</v>
+      </c>
+      <c r="K10" s="95" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="13" customFormat="1">
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="9">
+        <v>10</v>
+      </c>
+      <c r="C11" s="9">
+        <v>10</v>
+      </c>
+      <c r="D11" s="9">
+        <v>2</v>
+      </c>
+      <c r="E11" s="9">
+        <v>3</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="I11" s="10">
+        <v>4</v>
+      </c>
+      <c r="J11" s="10">
+        <v>5</v>
+      </c>
+      <c r="K11" s="95" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="13" customFormat="1">
+      <c r="A12" s="9">
+        <v>5</v>
+      </c>
+      <c r="B12" s="9">
+        <v>11</v>
+      </c>
+      <c r="C12" s="9">
+        <v>10</v>
+      </c>
+      <c r="D12" s="9">
+        <v>2</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="I12" s="10">
+        <v>4</v>
+      </c>
+      <c r="J12" s="10">
+        <v>5</v>
+      </c>
+      <c r="K12" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:12" s="13" customFormat="1">
+      <c r="A13" s="9">
+        <v>5</v>
+      </c>
+      <c r="B13" s="9">
+        <v>12</v>
+      </c>
+      <c r="C13" s="9">
+        <v>10</v>
+      </c>
+      <c r="D13" s="9">
+        <v>2</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="I13" s="10">
+        <v>4</v>
+      </c>
+      <c r="J13" s="10">
+        <v>5</v>
+      </c>
+      <c r="K13" s="95" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:12" s="13" customFormat="1">
+      <c r="A14" s="9">
+        <v>5</v>
+      </c>
+      <c r="B14" s="9">
+        <v>13</v>
+      </c>
+      <c r="C14" s="9">
+        <v>10</v>
+      </c>
+      <c r="D14" s="9">
+        <v>2</v>
+      </c>
+      <c r="E14" s="9">
+        <v>1</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="I14" s="10">
+        <v>4</v>
+      </c>
+      <c r="J14" s="10">
+        <v>5</v>
+      </c>
+      <c r="K14" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:12" s="13" customFormat="1">
+      <c r="A15" s="9">
+        <v>5</v>
+      </c>
+      <c r="B15" s="9">
+        <v>14</v>
+      </c>
+      <c r="C15" s="9">
+        <v>10</v>
+      </c>
+      <c r="D15" s="9">
+        <v>2</v>
+      </c>
+      <c r="E15" s="9">
+        <v>2</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="I15" s="10">
+        <v>4</v>
+      </c>
+      <c r="J15" s="10">
+        <v>5</v>
+      </c>
+      <c r="K15" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:12" s="13" customFormat="1">
+      <c r="A16" s="9">
+        <v>5</v>
+      </c>
+      <c r="B16" s="9">
+        <v>15</v>
+      </c>
+      <c r="C16" s="9">
+        <v>10</v>
+      </c>
+      <c r="D16" s="9">
+        <v>2</v>
+      </c>
+      <c r="E16" s="9">
+        <v>2</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="I16" s="10">
+        <v>4</v>
+      </c>
+      <c r="J16" s="10">
+        <v>5</v>
+      </c>
+      <c r="K16" s="95" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="13" customFormat="1">
+      <c r="A17" s="9">
+        <v>5</v>
+      </c>
+      <c r="B17" s="9">
+        <v>16</v>
+      </c>
+      <c r="C17" s="9">
+        <v>10</v>
+      </c>
+      <c r="D17" s="9">
+        <v>2</v>
+      </c>
+      <c r="E17" s="9">
+        <v>2</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="I17" s="10">
+        <v>4</v>
+      </c>
+      <c r="J17" s="10">
+        <v>5</v>
+      </c>
+      <c r="K17" s="95" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="13" customFormat="1">
+      <c r="A18" s="9">
+        <v>5</v>
+      </c>
+      <c r="B18" s="9">
+        <v>17</v>
+      </c>
+      <c r="C18" s="9">
+        <v>10</v>
+      </c>
+      <c r="D18" s="9">
+        <v>2</v>
+      </c>
+      <c r="E18" s="9">
+        <v>1</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="I18" s="10">
+        <v>4</v>
+      </c>
+      <c r="J18" s="10">
+        <v>5</v>
+      </c>
+      <c r="K18" s="95" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="30">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="I1" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="J1" s="76" t="s">
+        <v>326</v>
+      </c>
+      <c r="K1" s="58" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="7" customWidth="1"/>
+    <col min="11" max="11" width="30" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="91" customFormat="1" ht="35.25" customHeight="1">
+      <c r="A1" s="75" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="77" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="94" t="s">
+        <v>271</v>
+      </c>
+      <c r="G1" s="76" t="s">
+        <v>272</v>
+      </c>
+      <c r="H1" s="76" t="s">
+        <v>273</v>
+      </c>
+      <c r="I1" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="J1" s="76" t="s">
+        <v>326</v>
+      </c>
+      <c r="K1" s="76" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" s="79" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="90"/>
+    </row>
+    <row r="2" spans="1:13" s="52" customFormat="1" ht="30">
+      <c r="A2" s="92" t="s">
+        <v>337</v>
+      </c>
+      <c r="B2" s="49">
+        <v>1</v>
+      </c>
+      <c r="C2" s="49">
+        <v>8</v>
+      </c>
+      <c r="D2" s="50">
+        <v>1</v>
+      </c>
+      <c r="E2" s="49">
+        <v>1</v>
+      </c>
+      <c r="F2" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G2" s="51" t="s">
+        <v>338</v>
+      </c>
+      <c r="H2" s="70" t="s">
+        <v>339</v>
+      </c>
+      <c r="I2" s="50">
+        <v>1</v>
+      </c>
+      <c r="J2" s="50">
+        <v>2</v>
+      </c>
+      <c r="K2" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="49" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="52" customFormat="1" ht="30">
+      <c r="A3" s="92" t="s">
+        <v>337</v>
+      </c>
+      <c r="B3" s="49">
+        <v>2</v>
+      </c>
+      <c r="C3" s="49">
+        <v>8</v>
+      </c>
+      <c r="D3" s="50">
+        <v>1</v>
+      </c>
+      <c r="E3" s="49">
+        <v>1</v>
+      </c>
+      <c r="F3" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" s="51" t="s">
+        <v>338</v>
+      </c>
+      <c r="H3" s="53" t="s">
+        <v>339</v>
+      </c>
+      <c r="I3" s="49">
+        <v>1</v>
+      </c>
+      <c r="J3" s="49">
+        <v>2</v>
+      </c>
+      <c r="K3" s="53" t="s">
+        <v>331</v>
+      </c>
+      <c r="L3" s="49"/>
+    </row>
+    <row r="4" spans="1:13" s="52" customFormat="1" ht="30">
+      <c r="A4" s="92" t="s">
+        <v>337</v>
+      </c>
+      <c r="B4" s="49">
+        <v>3</v>
+      </c>
+      <c r="C4" s="49">
+        <v>0</v>
+      </c>
+      <c r="D4" s="50">
+        <v>1</v>
+      </c>
+      <c r="E4" s="49">
+        <v>2</v>
+      </c>
+      <c r="F4" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G4" s="51" t="s">
+        <v>338</v>
+      </c>
+      <c r="H4" s="93" t="s">
+        <v>341</v>
+      </c>
+      <c r="I4" s="49">
+        <v>1</v>
+      </c>
+      <c r="J4" s="49">
+        <v>1</v>
+      </c>
+      <c r="K4" s="51" t="s">
+        <v>332</v>
+      </c>
+      <c r="L4" s="49"/>
+    </row>
+    <row r="5" spans="1:13" s="52" customFormat="1" ht="30">
+      <c r="A5" s="92" t="s">
+        <v>337</v>
+      </c>
+      <c r="B5" s="49">
+        <v>3</v>
+      </c>
+      <c r="C5" s="49">
+        <v>0</v>
+      </c>
+      <c r="D5" s="50">
+        <v>1</v>
+      </c>
+      <c r="E5" s="49">
+        <v>2</v>
+      </c>
+      <c r="F5" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G5" s="51" t="s">
+        <v>338</v>
+      </c>
+      <c r="H5" s="70" t="s">
+        <v>339</v>
+      </c>
+      <c r="I5" s="49">
+        <v>1</v>
+      </c>
+      <c r="J5" s="49">
+        <v>2</v>
+      </c>
+      <c r="K5" s="51" t="s">
+        <v>332</v>
+      </c>
+      <c r="L5" s="49"/>
+    </row>
+    <row r="6" spans="1:13" s="52" customFormat="1" ht="30">
+      <c r="A6" s="92" t="s">
+        <v>337</v>
+      </c>
+      <c r="B6" s="49">
+        <v>4</v>
+      </c>
+      <c r="C6" s="49">
+        <v>10</v>
+      </c>
+      <c r="D6" s="50">
+        <v>1</v>
+      </c>
+      <c r="E6" s="49">
+        <v>1</v>
+      </c>
+      <c r="F6" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G6" s="51" t="s">
+        <v>338</v>
+      </c>
+      <c r="H6" s="70" t="s">
+        <v>339</v>
+      </c>
+      <c r="I6" s="49">
+        <v>1</v>
+      </c>
+      <c r="J6" s="49">
+        <v>2</v>
+      </c>
+      <c r="K6" s="51" t="s">
+        <v>333</v>
+      </c>
+      <c r="L6" s="49"/>
+    </row>
+    <row r="7" spans="1:13" s="52" customFormat="1">
+      <c r="A7" s="92" t="s">
+        <v>337</v>
+      </c>
+      <c r="B7" s="49">
+        <v>5</v>
+      </c>
+      <c r="C7" s="49">
+        <v>10</v>
+      </c>
+      <c r="D7" s="50">
+        <v>1</v>
+      </c>
+      <c r="E7" s="49">
+        <v>1</v>
+      </c>
+      <c r="F7" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G7" s="51" t="s">
+        <v>338</v>
+      </c>
+      <c r="H7" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="I7" s="49">
+        <v>1</v>
+      </c>
+      <c r="J7" s="49">
+        <v>3</v>
+      </c>
+      <c r="K7" s="51" t="s">
+        <v>334</v>
+      </c>
+      <c r="L7" s="49"/>
+    </row>
+    <row r="8" spans="1:13" s="52" customFormat="1" ht="30">
+      <c r="A8" s="92" t="s">
+        <v>337</v>
+      </c>
+      <c r="B8" s="49">
+        <v>6</v>
+      </c>
+      <c r="C8" s="49">
+        <v>10</v>
+      </c>
+      <c r="D8" s="50">
+        <v>1</v>
+      </c>
+      <c r="E8" s="49">
+        <v>1</v>
+      </c>
+      <c r="F8" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G8" s="51" t="s">
+        <v>338</v>
+      </c>
+      <c r="H8" s="70" t="s">
+        <v>339</v>
+      </c>
+      <c r="I8" s="49">
+        <v>1</v>
+      </c>
+      <c r="J8" s="49">
+        <v>2</v>
+      </c>
+      <c r="K8" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="L8" s="49"/>
+    </row>
+    <row r="9" spans="1:13" s="52" customFormat="1">
+      <c r="A9" s="92" t="s">
+        <v>337</v>
+      </c>
+      <c r="B9" s="49">
+        <v>7</v>
+      </c>
+      <c r="C9" s="49">
+        <v>10</v>
+      </c>
+      <c r="D9" s="50">
+        <v>1</v>
+      </c>
+      <c r="E9" s="49">
+        <v>2</v>
+      </c>
+      <c r="F9" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G9" s="51" t="s">
+        <v>338</v>
+      </c>
+      <c r="H9" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="I9" s="49">
+        <v>1</v>
+      </c>
+      <c r="J9" s="49">
+        <v>3</v>
+      </c>
+      <c r="K9" s="51" t="s">
+        <v>342</v>
+      </c>
+      <c r="L9" s="49"/>
+    </row>
+    <row r="10" spans="1:13" s="52" customFormat="1">
+      <c r="A10" s="92" t="s">
+        <v>337</v>
+      </c>
+      <c r="B10" s="49">
+        <v>8</v>
+      </c>
+      <c r="C10" s="49">
+        <v>5</v>
+      </c>
+      <c r="D10" s="50">
+        <v>1</v>
+      </c>
+      <c r="E10" s="49">
+        <v>3</v>
+      </c>
+      <c r="F10" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G10" s="51" t="s">
+        <v>338</v>
+      </c>
+      <c r="H10" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="I10" s="49">
+        <v>1</v>
+      </c>
+      <c r="J10" s="49">
+        <v>3</v>
+      </c>
+      <c r="K10" s="51" t="s">
+        <v>343</v>
+      </c>
+      <c r="L10" s="49"/>
+    </row>
+    <row r="11" spans="1:13" s="13" customFormat="1">
+      <c r="A11" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B11" s="9">
+        <v>9</v>
+      </c>
+      <c r="C11" s="9">
+        <v>10</v>
+      </c>
+      <c r="D11" s="10">
+        <v>1</v>
+      </c>
+      <c r="E11" s="9">
+        <v>2</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="I11" s="10">
+        <v>1</v>
+      </c>
+      <c r="J11" s="10">
+        <v>2</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:13" s="13" customFormat="1">
+      <c r="A12" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B12" s="9">
+        <v>10</v>
+      </c>
+      <c r="C12" s="9">
+        <v>10</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="9">
+        <v>2</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="I12" s="9">
+        <v>1</v>
+      </c>
+      <c r="J12" s="9">
+        <v>2</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:13" s="13" customFormat="1">
+      <c r="A13" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B13" s="9">
+        <v>11</v>
+      </c>
+      <c r="C13" s="9">
+        <v>10</v>
+      </c>
+      <c r="D13" s="10">
+        <v>1</v>
+      </c>
+      <c r="E13" s="9">
+        <v>3</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="I13" s="10">
+        <v>1</v>
+      </c>
+      <c r="J13" s="10">
+        <v>4</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="L13" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="55" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="I1" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="J1" s="76" t="s">
+        <v>326</v>
+      </c>
+      <c r="K1" s="58" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" s="56" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated questons and lists
</commit_message>
<xml_diff>
--- a/lists/lists.rs.xlsx
+++ b/lists/lists.rs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-90" windowWidth="15600" windowHeight="5190" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="-120" yWindow="-90" windowWidth="15600" windowHeight="5190" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="fractions" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2473" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2494" uniqueCount="363">
   <si>
     <t>RAZRED</t>
   </si>
@@ -1210,6 +1210,21 @@
   </si>
   <si>
     <t>fract.38</t>
+  </si>
+  <si>
+    <t>Prosti i složeni brojevi</t>
+  </si>
+  <si>
+    <t>Rastavljanje na proste činioce</t>
+  </si>
+  <si>
+    <t>Erastotenovo sito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ivice - površina  </t>
+  </si>
+  <si>
+    <t>Sabiranje I oduzimanje</t>
   </si>
 </sst>
 </file>
@@ -1396,7 +1411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1637,6 +1652,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1947,7 +1968,7 @@
   <dimension ref="A1:L69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
@@ -4311,7 +4332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -4376,8 +4397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="E1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -7689,7 +7710,7 @@
   <dimension ref="A1:M251"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A208" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -18690,11 +18711,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L112"/>
+  <dimension ref="A1:L115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L115" sqref="L115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22790,6 +22811,120 @@
       </c>
       <c r="L112" s="34"/>
     </row>
+    <row r="113" spans="1:12" s="45" customFormat="1">
+      <c r="A113" s="42">
+        <v>4</v>
+      </c>
+      <c r="B113" s="42">
+        <v>100</v>
+      </c>
+      <c r="C113" s="42">
+        <v>10</v>
+      </c>
+      <c r="D113" s="43">
+        <v>1</v>
+      </c>
+      <c r="E113" s="42">
+        <v>3</v>
+      </c>
+      <c r="F113" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="G113" s="44" t="s">
+        <v>239</v>
+      </c>
+      <c r="H113" s="44" t="s">
+        <v>240</v>
+      </c>
+      <c r="I113" s="42">
+        <v>3</v>
+      </c>
+      <c r="J113" s="42">
+        <v>2</v>
+      </c>
+      <c r="K113" s="60" t="s">
+        <v>242</v>
+      </c>
+      <c r="L113" s="42">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" s="45" customFormat="1">
+      <c r="A114" s="42">
+        <v>4</v>
+      </c>
+      <c r="B114" s="42">
+        <v>101</v>
+      </c>
+      <c r="C114" s="42">
+        <v>10</v>
+      </c>
+      <c r="D114" s="43">
+        <v>1</v>
+      </c>
+      <c r="E114" s="42">
+        <v>3</v>
+      </c>
+      <c r="F114" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="G114" s="44" t="s">
+        <v>239</v>
+      </c>
+      <c r="H114" s="44" t="s">
+        <v>240</v>
+      </c>
+      <c r="I114" s="42">
+        <v>3</v>
+      </c>
+      <c r="J114" s="42">
+        <v>2</v>
+      </c>
+      <c r="K114" s="60" t="s">
+        <v>361</v>
+      </c>
+      <c r="L114" s="42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" s="45" customFormat="1">
+      <c r="A115" s="42">
+        <v>4</v>
+      </c>
+      <c r="B115" s="42">
+        <v>102</v>
+      </c>
+      <c r="C115" s="42">
+        <v>10</v>
+      </c>
+      <c r="D115" s="43">
+        <v>1</v>
+      </c>
+      <c r="E115" s="42">
+        <v>2</v>
+      </c>
+      <c r="F115" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="G115" s="44" t="s">
+        <v>244</v>
+      </c>
+      <c r="H115" s="44" t="s">
+        <v>246</v>
+      </c>
+      <c r="I115" s="42">
+        <v>5</v>
+      </c>
+      <c r="J115" s="42">
+        <v>2</v>
+      </c>
+      <c r="K115" s="60" t="s">
+        <v>242</v>
+      </c>
+      <c r="L115" s="42">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -22798,10 +22933,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22811,7 +22946,7 @@
     <col min="6" max="6" width="15.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="55" customFormat="1" ht="30">
@@ -22957,7 +23092,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="13" customFormat="1" ht="28.5" customHeight="1">
+    <row r="5" spans="1:12" s="13" customFormat="1" ht="27" customHeight="1">
       <c r="A5" s="9">
         <v>5</v>
       </c>
@@ -22989,7 +23124,7 @@
         <v>2</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="13" customFormat="1" ht="27" customHeight="1">
@@ -23131,6 +23266,9 @@
       <c r="K9" s="12" t="s">
         <v>353</v>
       </c>
+      <c r="L9" s="9">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:12" s="13" customFormat="1">
       <c r="A10" s="9">
@@ -23455,6 +23593,41 @@
       </c>
       <c r="K18" s="95" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="13" customFormat="1">
+      <c r="A19" s="9">
+        <v>5</v>
+      </c>
+      <c r="B19" s="9">
+        <v>18</v>
+      </c>
+      <c r="C19" s="9">
+        <v>10</v>
+      </c>
+      <c r="D19" s="9">
+        <v>2</v>
+      </c>
+      <c r="E19" s="9">
+        <v>1</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="I19" s="10">
+        <v>4</v>
+      </c>
+      <c r="J19" s="10">
+        <v>5</v>
+      </c>
+      <c r="K19" s="95" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -23528,10 +23701,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24021,6 +24194,42 @@
         <v>336</v>
       </c>
       <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:13" s="13" customFormat="1" ht="30" customHeight="1">
+      <c r="A14" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B14" s="9">
+        <v>12</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10">
+        <v>2</v>
+      </c>
+      <c r="E14" s="9">
+        <v>2</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" s="97" t="s">
+        <v>358</v>
+      </c>
+      <c r="H14" s="98" t="s">
+        <v>359</v>
+      </c>
+      <c r="I14" s="10">
+        <v>3</v>
+      </c>
+      <c r="J14" s="10">
+        <v>1</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="L14" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New questions and lists
</commit_message>
<xml_diff>
--- a/lists/lists.rs.xlsx
+++ b/lists/lists.rs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-90" windowWidth="15600" windowHeight="5190" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-90" windowWidth="15600" windowHeight="5190" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="fractions" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2605" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2674" uniqueCount="395">
   <si>
     <t>RAZRED</t>
   </si>
@@ -1291,6 +1291,36 @@
   </si>
   <si>
     <t>Najmanji zajednički sadržalac tri broja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tekstualni zadatak </t>
+  </si>
+  <si>
+    <t>Svi  dvocifreni sadržaoci  jednog broja</t>
+  </si>
+  <si>
+    <t>Tekstualni zadatak - najveći delilac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tekstualni zadatak -najmanji  sadržalac </t>
+  </si>
+  <si>
+    <t>Najmanji  sadržalac - nepoznati činilac</t>
+  </si>
+  <si>
+    <t>Skupovi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Različiti zapisi skupa </t>
+  </si>
+  <si>
+    <t>Složena figura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jednaki skupovi, podskup </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broj elemenata skupa </t>
   </si>
 </sst>
 </file>
@@ -1477,7 +1507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1725,6 +1755,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4465,8 +4501,8 @@
   <dimension ref="A1:L93"/>
   <sheetViews>
     <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4477,7 +4513,7 @@
     <col min="5" max="5" width="8.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" style="4" customWidth="1"/>
     <col min="7" max="7" width="24.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="27.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="32" style="2" customWidth="1"/>
     <col min="9" max="10" width="7.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="29.28515625" style="2" customWidth="1"/>
     <col min="12" max="12" width="10.85546875" style="1" customWidth="1"/>
@@ -18892,11 +18928,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L115"/>
+  <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L117" sqref="L117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23104,6 +23140,82 @@
       </c>
       <c r="L115" s="42">
         <v>80</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" s="38" customFormat="1">
+      <c r="A116" s="34">
+        <v>3</v>
+      </c>
+      <c r="B116" s="34">
+        <v>103</v>
+      </c>
+      <c r="C116" s="34">
+        <v>8</v>
+      </c>
+      <c r="D116" s="35">
+        <v>2</v>
+      </c>
+      <c r="E116" s="34">
+        <v>2</v>
+      </c>
+      <c r="F116" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G116" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="H116" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="I116" s="34">
+        <v>1</v>
+      </c>
+      <c r="J116" s="34">
+        <v>2</v>
+      </c>
+      <c r="K116" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="L116" s="34">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" s="45" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A117" s="42">
+        <v>4</v>
+      </c>
+      <c r="B117" s="42">
+        <v>104</v>
+      </c>
+      <c r="C117" s="42">
+        <v>10</v>
+      </c>
+      <c r="D117" s="43">
+        <v>1</v>
+      </c>
+      <c r="E117" s="42">
+        <v>2</v>
+      </c>
+      <c r="F117" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="G117" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="H117" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="I117" s="43">
+        <v>2</v>
+      </c>
+      <c r="J117" s="42">
+        <v>2</v>
+      </c>
+      <c r="K117" s="100" t="s">
+        <v>392</v>
+      </c>
+      <c r="L117" s="101">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -23882,10 +23994,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24878,7 +24990,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>91</v>
@@ -24914,7 +25026,7 @@
         <v>2</v>
       </c>
       <c r="E28" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>91</v>
@@ -24990,7 +25102,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>91</v>
@@ -25028,7 +25140,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>91</v>
@@ -25088,6 +25200,458 @@
       </c>
       <c r="L32" s="9">
         <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="13" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A33" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B33" s="9">
+        <v>31</v>
+      </c>
+      <c r="C33" s="9">
+        <v>6</v>
+      </c>
+      <c r="D33" s="10">
+        <v>1</v>
+      </c>
+      <c r="E33" s="9">
+        <v>2</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="I33" s="10">
+        <v>1</v>
+      </c>
+      <c r="J33" s="10">
+        <v>2</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="L33" s="9" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="13" customFormat="1">
+      <c r="A34" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B34" s="9">
+        <v>32</v>
+      </c>
+      <c r="C34" s="9">
+        <v>10</v>
+      </c>
+      <c r="D34" s="10">
+        <v>2</v>
+      </c>
+      <c r="E34" s="9">
+        <v>2</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="I34" s="9">
+        <v>1</v>
+      </c>
+      <c r="J34" s="9">
+        <v>5</v>
+      </c>
+      <c r="K34" s="12" t="s">
+        <v>387</v>
+      </c>
+      <c r="L34" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="13" customFormat="1">
+      <c r="A35" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B35" s="9">
+        <v>33</v>
+      </c>
+      <c r="C35" s="9">
+        <v>10</v>
+      </c>
+      <c r="D35" s="10">
+        <v>1</v>
+      </c>
+      <c r="E35" s="9">
+        <v>1</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="I35" s="10">
+        <v>1</v>
+      </c>
+      <c r="J35" s="10">
+        <v>2</v>
+      </c>
+      <c r="K35" s="12" t="s">
+        <v>386</v>
+      </c>
+      <c r="L35" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" s="13" customFormat="1">
+      <c r="A36" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B36" s="9">
+        <v>34</v>
+      </c>
+      <c r="C36" s="9">
+        <v>10</v>
+      </c>
+      <c r="D36" s="10">
+        <v>2</v>
+      </c>
+      <c r="E36" s="9">
+        <v>3</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="I36" s="9">
+        <v>1</v>
+      </c>
+      <c r="J36" s="9">
+        <v>5</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>387</v>
+      </c>
+      <c r="L36" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="13" customFormat="1">
+      <c r="A37" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B37" s="9">
+        <v>35</v>
+      </c>
+      <c r="C37" s="9">
+        <v>10</v>
+      </c>
+      <c r="D37" s="10">
+        <v>2</v>
+      </c>
+      <c r="E37" s="9">
+        <v>3</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="I37" s="9">
+        <v>1</v>
+      </c>
+      <c r="J37" s="9">
+        <v>5</v>
+      </c>
+      <c r="K37" s="11" t="s">
+        <v>388</v>
+      </c>
+      <c r="L37" s="9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="13" customFormat="1">
+      <c r="A38" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B38" s="9">
+        <v>36</v>
+      </c>
+      <c r="C38" s="9">
+        <v>10</v>
+      </c>
+      <c r="D38" s="10">
+        <v>2</v>
+      </c>
+      <c r="E38" s="9">
+        <v>2</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="I38" s="9">
+        <v>1</v>
+      </c>
+      <c r="J38" s="9">
+        <v>5</v>
+      </c>
+      <c r="K38" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="L38" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="13" customFormat="1">
+      <c r="A39" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B39" s="9">
+        <v>37</v>
+      </c>
+      <c r="C39" s="9">
+        <v>8</v>
+      </c>
+      <c r="D39" s="10">
+        <v>1</v>
+      </c>
+      <c r="E39" s="9">
+        <v>1</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I39" s="9">
+        <v>2</v>
+      </c>
+      <c r="J39" s="9">
+        <v>1</v>
+      </c>
+      <c r="K39" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="L39" s="9"/>
+    </row>
+    <row r="40" spans="1:12" s="13" customFormat="1">
+      <c r="A40" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B40" s="9">
+        <v>38</v>
+      </c>
+      <c r="C40" s="9">
+        <v>6</v>
+      </c>
+      <c r="D40" s="10">
+        <v>1</v>
+      </c>
+      <c r="E40" s="9">
+        <v>1</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I40" s="9">
+        <v>2</v>
+      </c>
+      <c r="J40" s="9">
+        <v>1</v>
+      </c>
+      <c r="K40" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="L40" s="9">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="13" customFormat="1">
+      <c r="A41" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B41" s="9">
+        <v>39</v>
+      </c>
+      <c r="C41" s="9">
+        <v>8</v>
+      </c>
+      <c r="D41" s="10">
+        <v>1</v>
+      </c>
+      <c r="E41" s="9">
+        <v>1</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I41" s="9">
+        <v>2</v>
+      </c>
+      <c r="J41" s="9">
+        <v>1</v>
+      </c>
+      <c r="K41" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="L41" s="9">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="13" customFormat="1">
+      <c r="A42" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B42" s="9">
+        <v>40</v>
+      </c>
+      <c r="C42" s="9">
+        <v>0</v>
+      </c>
+      <c r="D42" s="10">
+        <v>1</v>
+      </c>
+      <c r="E42" s="9">
+        <v>1</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I42" s="9">
+        <v>2</v>
+      </c>
+      <c r="J42" s="9">
+        <v>1</v>
+      </c>
+      <c r="K42" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="L42" s="9">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" s="13" customFormat="1">
+      <c r="A43" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B43" s="9">
+        <v>41</v>
+      </c>
+      <c r="C43" s="9">
+        <v>8</v>
+      </c>
+      <c r="D43" s="10">
+        <v>1</v>
+      </c>
+      <c r="E43" s="9">
+        <v>2</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I43" s="9">
+        <v>2</v>
+      </c>
+      <c r="J43" s="9">
+        <v>1</v>
+      </c>
+      <c r="K43" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="L43" s="9"/>
+    </row>
+    <row r="44" spans="1:12" s="13" customFormat="1">
+      <c r="A44" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B44" s="9">
+        <v>42</v>
+      </c>
+      <c r="C44" s="9">
+        <v>8</v>
+      </c>
+      <c r="D44" s="10">
+        <v>1</v>
+      </c>
+      <c r="E44" s="9">
+        <v>2</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I44" s="9">
+        <v>2</v>
+      </c>
+      <c r="J44" s="9">
+        <v>1</v>
+      </c>
+      <c r="K44" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="L44" s="9">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new questions and lists
</commit_message>
<xml_diff>
--- a/lists/lists.rs.xlsx
+++ b/lists/lists.rs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="15600" windowHeight="11760" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="15600" windowHeight="11760" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="fractions" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3120" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3164" uniqueCount="507">
   <si>
     <t>RAZRED</t>
   </si>
@@ -1646,6 +1646,30 @@
   </si>
   <si>
     <t>fract_2 9</t>
+  </si>
+  <si>
+    <t>jednačine</t>
+  </si>
+  <si>
+    <t>fract_2 39</t>
+  </si>
+  <si>
+    <t>fract_2 54</t>
+  </si>
+  <si>
+    <t>množenje I br.prava</t>
+  </si>
+  <si>
+    <t>fract_2 22</t>
+  </si>
+  <si>
+    <t>deljenje I br.prava</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linearna </t>
+  </si>
+  <si>
+    <t>prirodni broj</t>
   </si>
 </sst>
 </file>
@@ -1832,7 +1856,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2111,9 +2135,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -5005,10 +5026,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD41"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6670,6 +6691,45 @@
       <c r="M41" s="9">
         <v>35</v>
       </c>
+    </row>
+    <row r="42" spans="1:13" s="13" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A42" s="9">
+        <v>5</v>
+      </c>
+      <c r="B42" s="9">
+        <v>37</v>
+      </c>
+      <c r="C42" s="9">
+        <v>10</v>
+      </c>
+      <c r="D42" s="9">
+        <v>3</v>
+      </c>
+      <c r="E42" s="9">
+        <v>3</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>457</v>
+      </c>
+      <c r="I42" s="10">
+        <v>4</v>
+      </c>
+      <c r="J42" s="10">
+        <v>1</v>
+      </c>
+      <c r="K42" s="10">
+        <v>1</v>
+      </c>
+      <c r="L42" s="111" t="s">
+        <v>499</v>
+      </c>
+      <c r="M42" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10274,7 +10334,7 @@
   <dimension ref="A1:N255"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A235" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I127" sqref="I127"/>
     </sheetView>
   </sheetViews>
@@ -29534,7 +29594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -31883,10 +31943,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -31896,7 +31956,7 @@
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" customWidth="1"/>
     <col min="8" max="8" width="27.140625" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" customWidth="1"/>
@@ -31982,7 +32042,7 @@
       <c r="K2" s="10">
         <v>1</v>
       </c>
-      <c r="L2" s="112" t="s">
+      <c r="L2" s="111" t="s">
         <v>490</v>
       </c>
       <c r="M2" s="9" t="s">
@@ -32023,7 +32083,7 @@
       <c r="K3" s="10">
         <v>1</v>
       </c>
-      <c r="L3" s="112" t="s">
+      <c r="L3" s="111" t="s">
         <v>491</v>
       </c>
       <c r="M3" s="9" t="s">
@@ -32064,7 +32124,7 @@
       <c r="K4" s="10">
         <v>1</v>
       </c>
-      <c r="L4" s="112" t="s">
+      <c r="L4" s="111" t="s">
         <v>493</v>
       </c>
       <c r="M4" s="9">
@@ -32105,7 +32165,7 @@
       <c r="K5" s="10">
         <v>1</v>
       </c>
-      <c r="L5" s="112" t="s">
+      <c r="L5" s="111" t="s">
         <v>494</v>
       </c>
       <c r="M5" s="9">
@@ -32146,7 +32206,7 @@
       <c r="K6" s="10">
         <v>1</v>
       </c>
-      <c r="L6" s="112" t="s">
+      <c r="L6" s="111" t="s">
         <v>495</v>
       </c>
       <c r="M6" s="9">
@@ -32187,7 +32247,7 @@
       <c r="K7" s="10">
         <v>1</v>
       </c>
-      <c r="L7" s="112" t="s">
+      <c r="L7" s="111" t="s">
         <v>496</v>
       </c>
       <c r="M7" s="9" t="s">
@@ -32228,15 +32288,381 @@
       <c r="K8" s="10">
         <v>1</v>
       </c>
-      <c r="L8" s="112" t="s">
+      <c r="L8" s="111" t="s">
         <v>224</v>
       </c>
       <c r="M8" s="9" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
-      <c r="H10" s="111"/>
+    <row r="9" spans="1:13" s="13" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A9" s="9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="9">
+        <v>10</v>
+      </c>
+      <c r="D9" s="9">
+        <v>2</v>
+      </c>
+      <c r="E9" s="9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="I9" s="9">
+        <v>2</v>
+      </c>
+      <c r="J9" s="10">
+        <v>1</v>
+      </c>
+      <c r="K9" s="10">
+        <v>1</v>
+      </c>
+      <c r="L9" s="111" t="s">
+        <v>224</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="13" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A10" s="9">
+        <v>5</v>
+      </c>
+      <c r="B10" s="9">
+        <v>9</v>
+      </c>
+      <c r="C10" s="9">
+        <v>10</v>
+      </c>
+      <c r="D10" s="9">
+        <v>2</v>
+      </c>
+      <c r="E10" s="9">
+        <v>2</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="I10" s="9">
+        <v>2</v>
+      </c>
+      <c r="J10" s="10">
+        <v>1</v>
+      </c>
+      <c r="K10" s="10">
+        <v>1</v>
+      </c>
+      <c r="L10" s="111" t="s">
+        <v>224</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="13" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="9">
+        <v>10</v>
+      </c>
+      <c r="C11" s="9">
+        <v>10</v>
+      </c>
+      <c r="D11" s="9">
+        <v>2</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="I11" s="9">
+        <v>2</v>
+      </c>
+      <c r="J11" s="10">
+        <v>2</v>
+      </c>
+      <c r="K11" s="10">
+        <v>1</v>
+      </c>
+      <c r="L11" s="111" t="s">
+        <v>491</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="13" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A12" s="9">
+        <v>5</v>
+      </c>
+      <c r="B12" s="9">
+        <v>11</v>
+      </c>
+      <c r="C12" s="9">
+        <v>10</v>
+      </c>
+      <c r="D12" s="9">
+        <v>2</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="I12" s="9">
+        <v>2</v>
+      </c>
+      <c r="J12" s="10">
+        <v>2</v>
+      </c>
+      <c r="K12" s="10">
+        <v>1</v>
+      </c>
+      <c r="L12" s="111" t="s">
+        <v>493</v>
+      </c>
+      <c r="M12" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="13" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A13" s="9">
+        <v>5</v>
+      </c>
+      <c r="B13" s="9">
+        <v>12</v>
+      </c>
+      <c r="C13" s="9">
+        <v>10</v>
+      </c>
+      <c r="D13" s="9">
+        <v>2</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="I13" s="9">
+        <v>2</v>
+      </c>
+      <c r="J13" s="10">
+        <v>2</v>
+      </c>
+      <c r="K13" s="10">
+        <v>1</v>
+      </c>
+      <c r="L13" s="111" t="s">
+        <v>502</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="13" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A14" s="9">
+        <v>5</v>
+      </c>
+      <c r="B14" s="9">
+        <v>13</v>
+      </c>
+      <c r="C14" s="9">
+        <v>10</v>
+      </c>
+      <c r="D14" s="9">
+        <v>2</v>
+      </c>
+      <c r="E14" s="9">
+        <v>1</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="I14" s="9">
+        <v>2</v>
+      </c>
+      <c r="J14" s="10">
+        <v>2</v>
+      </c>
+      <c r="K14" s="10">
+        <v>1</v>
+      </c>
+      <c r="L14" s="111" t="s">
+        <v>504</v>
+      </c>
+      <c r="M14" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="13" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A15" s="9">
+        <v>5</v>
+      </c>
+      <c r="B15" s="9">
+        <v>14</v>
+      </c>
+      <c r="C15" s="9">
+        <v>10</v>
+      </c>
+      <c r="D15" s="9">
+        <v>2</v>
+      </c>
+      <c r="E15" s="9">
+        <v>2</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="I15" s="9">
+        <v>2</v>
+      </c>
+      <c r="J15" s="10">
+        <v>2</v>
+      </c>
+      <c r="K15" s="10">
+        <v>1</v>
+      </c>
+      <c r="L15" s="111" t="s">
+        <v>505</v>
+      </c>
+      <c r="M15" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="13" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A16" s="9">
+        <v>5</v>
+      </c>
+      <c r="B16" s="9">
+        <v>15</v>
+      </c>
+      <c r="C16" s="9">
+        <v>10</v>
+      </c>
+      <c r="D16" s="9">
+        <v>2</v>
+      </c>
+      <c r="E16" s="9">
+        <v>3</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="I16" s="9">
+        <v>2</v>
+      </c>
+      <c r="J16" s="10">
+        <v>2</v>
+      </c>
+      <c r="K16" s="10">
+        <v>1</v>
+      </c>
+      <c r="L16" s="111" t="s">
+        <v>224</v>
+      </c>
+      <c r="M16" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="13" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A17" s="9">
+        <v>5</v>
+      </c>
+      <c r="B17" s="9">
+        <v>16</v>
+      </c>
+      <c r="C17" s="9">
+        <v>10</v>
+      </c>
+      <c r="D17" s="9">
+        <v>2</v>
+      </c>
+      <c r="E17" s="9">
+        <v>2</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="I17" s="9">
+        <v>2</v>
+      </c>
+      <c r="J17" s="10">
+        <v>2</v>
+      </c>
+      <c r="K17" s="10">
+        <v>1</v>
+      </c>
+      <c r="L17" s="111" t="s">
+        <v>506</v>
+      </c>
+      <c r="M17" s="9">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New lists and questions
</commit_message>
<xml_diff>
--- a/lists/lists.rs.xlsx
+++ b/lists/lists.rs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="15600" windowHeight="11760" activeTab="6"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="15600" windowHeight="11760" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="fractions" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3596" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3736" uniqueCount="640">
   <si>
     <t>RAZRED</t>
   </si>
@@ -1982,6 +1982,93 @@
   </si>
   <si>
     <t>figura sa normalnim dijagonalama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">složena figura </t>
+  </si>
+  <si>
+    <t>Apsolutna vrednost</t>
+  </si>
+  <si>
+    <t>Suprotan broj, apsolutna vrednost</t>
+  </si>
+  <si>
+    <t>numbers 42</t>
+  </si>
+  <si>
+    <t>Zbir - tabela</t>
+  </si>
+  <si>
+    <t>Razlika - tabela</t>
+  </si>
+  <si>
+    <t>numbers 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zbir/razlika </t>
+  </si>
+  <si>
+    <t>numbers 187</t>
+  </si>
+  <si>
+    <t>Zbir/razlika, poređenje rezultata</t>
+  </si>
+  <si>
+    <t>numbers 39</t>
+  </si>
+  <si>
+    <t>sabiranje</t>
+  </si>
+  <si>
+    <t>numbers 181</t>
+  </si>
+  <si>
+    <t>pitanja</t>
+  </si>
+  <si>
+    <t>Množenje - tabela</t>
+  </si>
+  <si>
+    <t>numbers 90</t>
+  </si>
+  <si>
+    <t>Deljenje - tabela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sve računske operacije - tekst </t>
+  </si>
+  <si>
+    <t>numbers 94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sve računske operacije </t>
+  </si>
+  <si>
+    <t>numbers 93</t>
+  </si>
+  <si>
+    <t>numbers 63</t>
+  </si>
+  <si>
+    <t>Sa celim brojevima</t>
+  </si>
+  <si>
+    <t>equations 6</t>
+  </si>
+  <si>
+    <t>equations 16</t>
+  </si>
+  <si>
+    <t>Racionalni brojevi</t>
+  </si>
+  <si>
+    <t>decimalni I razlomci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojam, prikaz na brojevnoj pravoj </t>
+  </si>
+  <si>
+    <t>zapis tacaka na brojevnoj pravoj</t>
   </si>
 </sst>
 </file>
@@ -27397,10 +27484,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M61"/>
+  <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="I46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M67" sqref="M67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27408,7 +27495,7 @@
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="7.28515625" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
     <col min="8" max="8" width="36" customWidth="1"/>
     <col min="9" max="9" width="8.5703125" customWidth="1"/>
     <col min="12" max="12" width="26.7109375" customWidth="1"/>
@@ -29878,6 +29965,129 @@
         <v>31</v>
       </c>
     </row>
+    <row r="62" spans="1:13" s="52" customFormat="1">
+      <c r="A62" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B62" s="49">
+        <v>61</v>
+      </c>
+      <c r="C62" s="49">
+        <v>10</v>
+      </c>
+      <c r="D62" s="50">
+        <v>2</v>
+      </c>
+      <c r="E62" s="49">
+        <v>1</v>
+      </c>
+      <c r="F62" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G62" s="51" t="s">
+        <v>636</v>
+      </c>
+      <c r="H62" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I62" s="50">
+        <v>1</v>
+      </c>
+      <c r="J62" s="49">
+        <v>2</v>
+      </c>
+      <c r="K62" s="49">
+        <v>2</v>
+      </c>
+      <c r="L62" s="51" t="s">
+        <v>637</v>
+      </c>
+      <c r="M62" s="49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" s="52" customFormat="1">
+      <c r="A63" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B63" s="49">
+        <v>62</v>
+      </c>
+      <c r="C63" s="49">
+        <v>10</v>
+      </c>
+      <c r="D63" s="50">
+        <v>2</v>
+      </c>
+      <c r="E63" s="49">
+        <v>2</v>
+      </c>
+      <c r="F63" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G63" s="51" t="s">
+        <v>636</v>
+      </c>
+      <c r="H63" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I63" s="50">
+        <v>1</v>
+      </c>
+      <c r="J63" s="49">
+        <v>2</v>
+      </c>
+      <c r="K63" s="49">
+        <v>2</v>
+      </c>
+      <c r="L63" s="51" t="s">
+        <v>637</v>
+      </c>
+      <c r="M63" s="49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" s="52" customFormat="1">
+      <c r="A64" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B64" s="49">
+        <v>63</v>
+      </c>
+      <c r="C64" s="49">
+        <v>10</v>
+      </c>
+      <c r="D64" s="50">
+        <v>2</v>
+      </c>
+      <c r="E64" s="49">
+        <v>1</v>
+      </c>
+      <c r="F64" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G64" s="51" t="s">
+        <v>636</v>
+      </c>
+      <c r="H64" s="52" t="s">
+        <v>638</v>
+      </c>
+      <c r="I64" s="50">
+        <v>1</v>
+      </c>
+      <c r="J64" s="49">
+        <v>2</v>
+      </c>
+      <c r="K64" s="49">
+        <v>1</v>
+      </c>
+      <c r="L64" s="51" t="s">
+        <v>639</v>
+      </c>
+      <c r="M64" s="49">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -29886,10 +30096,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M100"/>
+  <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="M100" sqref="M100"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -33973,6 +34183,88 @@
         <v>95</v>
       </c>
     </row>
+    <row r="101" spans="1:13" s="18" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A101" s="15">
+        <v>6</v>
+      </c>
+      <c r="B101" s="15">
+        <v>99</v>
+      </c>
+      <c r="C101" s="15">
+        <v>8</v>
+      </c>
+      <c r="D101" s="16">
+        <v>3</v>
+      </c>
+      <c r="E101" s="15">
+        <v>2</v>
+      </c>
+      <c r="F101" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="G101" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="H101" s="65" t="s">
+        <v>608</v>
+      </c>
+      <c r="I101" s="16">
+        <v>3</v>
+      </c>
+      <c r="J101" s="83">
+        <v>3</v>
+      </c>
+      <c r="K101" s="83">
+        <v>3</v>
+      </c>
+      <c r="L101" s="65" t="s">
+        <v>611</v>
+      </c>
+      <c r="M101" s="15">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" s="18" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A102" s="15">
+        <v>6</v>
+      </c>
+      <c r="B102" s="15">
+        <v>100</v>
+      </c>
+      <c r="C102" s="15">
+        <v>8</v>
+      </c>
+      <c r="D102" s="16">
+        <v>3</v>
+      </c>
+      <c r="E102" s="15">
+        <v>3</v>
+      </c>
+      <c r="F102" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="G102" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="H102" s="65" t="s">
+        <v>608</v>
+      </c>
+      <c r="I102" s="16">
+        <v>3</v>
+      </c>
+      <c r="J102" s="83">
+        <v>3</v>
+      </c>
+      <c r="K102" s="83">
+        <v>3</v>
+      </c>
+      <c r="L102" s="65" t="s">
+        <v>611</v>
+      </c>
+      <c r="M102" s="15">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -33981,10 +34273,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N58"/>
+  <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77:XFD77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34334,7 +34626,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" s="53" t="s">
         <v>178</v>
@@ -36319,6 +36611,785 @@
       </c>
       <c r="M58" s="9">
         <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" s="52" customFormat="1" ht="30">
+      <c r="A59" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B59" s="49">
+        <v>57</v>
+      </c>
+      <c r="C59" s="49">
+        <v>10</v>
+      </c>
+      <c r="D59" s="50">
+        <v>1</v>
+      </c>
+      <c r="E59" s="49">
+        <v>1</v>
+      </c>
+      <c r="F59" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G59" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H59" s="91" t="s">
+        <v>340</v>
+      </c>
+      <c r="I59" s="50">
+        <v>1</v>
+      </c>
+      <c r="J59" s="49">
+        <v>1</v>
+      </c>
+      <c r="K59" s="49">
+        <v>1</v>
+      </c>
+      <c r="L59" s="51" t="s">
+        <v>612</v>
+      </c>
+      <c r="M59" s="49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" s="52" customFormat="1" ht="30">
+      <c r="A60" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B60" s="49">
+        <v>57</v>
+      </c>
+      <c r="C60" s="49">
+        <v>10</v>
+      </c>
+      <c r="D60" s="50">
+        <v>1</v>
+      </c>
+      <c r="E60" s="49">
+        <v>1</v>
+      </c>
+      <c r="F60" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G60" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H60" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="I60" s="50">
+        <v>1</v>
+      </c>
+      <c r="J60" s="49">
+        <v>1</v>
+      </c>
+      <c r="K60" s="49">
+        <v>2</v>
+      </c>
+      <c r="L60" s="51" t="s">
+        <v>350</v>
+      </c>
+      <c r="M60" s="49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" s="52" customFormat="1" ht="30">
+      <c r="A61" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B61" s="49">
+        <v>58</v>
+      </c>
+      <c r="C61" s="49">
+        <v>10</v>
+      </c>
+      <c r="D61" s="50">
+        <v>1</v>
+      </c>
+      <c r="E61" s="49">
+        <v>2</v>
+      </c>
+      <c r="F61" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G61" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H61" s="91" t="s">
+        <v>340</v>
+      </c>
+      <c r="I61" s="50">
+        <v>1</v>
+      </c>
+      <c r="J61" s="49">
+        <v>1</v>
+      </c>
+      <c r="K61" s="49">
+        <v>1</v>
+      </c>
+      <c r="L61" s="51" t="s">
+        <v>612</v>
+      </c>
+      <c r="M61" s="49">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" s="52" customFormat="1" ht="30">
+      <c r="A62" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B62" s="49">
+        <v>58</v>
+      </c>
+      <c r="C62" s="49">
+        <v>10</v>
+      </c>
+      <c r="D62" s="50">
+        <v>1</v>
+      </c>
+      <c r="E62" s="49">
+        <v>2</v>
+      </c>
+      <c r="F62" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G62" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H62" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="I62" s="50">
+        <v>1</v>
+      </c>
+      <c r="J62" s="49">
+        <v>1</v>
+      </c>
+      <c r="K62" s="49">
+        <v>2</v>
+      </c>
+      <c r="L62" s="51" t="s">
+        <v>350</v>
+      </c>
+      <c r="M62" s="49">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" s="52" customFormat="1" ht="30">
+      <c r="A63" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B63" s="49">
+        <v>59</v>
+      </c>
+      <c r="C63" s="49">
+        <v>10</v>
+      </c>
+      <c r="D63" s="50">
+        <v>1</v>
+      </c>
+      <c r="E63" s="49">
+        <v>2</v>
+      </c>
+      <c r="F63" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G63" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H63" s="91" t="s">
+        <v>340</v>
+      </c>
+      <c r="I63" s="50">
+        <v>1</v>
+      </c>
+      <c r="J63" s="49">
+        <v>1</v>
+      </c>
+      <c r="K63" s="49">
+        <v>1</v>
+      </c>
+      <c r="L63" s="51" t="s">
+        <v>613</v>
+      </c>
+      <c r="M63" s="49">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" s="52" customFormat="1">
+      <c r="A64" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B64" s="49">
+        <v>60</v>
+      </c>
+      <c r="C64" s="49">
+        <v>10</v>
+      </c>
+      <c r="D64" s="50">
+        <v>1</v>
+      </c>
+      <c r="E64" s="49">
+        <v>1</v>
+      </c>
+      <c r="F64" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G64" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H64" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="I64" s="50">
+        <v>1</v>
+      </c>
+      <c r="J64" s="49">
+        <v>1</v>
+      </c>
+      <c r="K64" s="49">
+        <v>3</v>
+      </c>
+      <c r="L64" s="51" t="s">
+        <v>615</v>
+      </c>
+      <c r="M64" s="49" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" s="52" customFormat="1">
+      <c r="A65" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B65" s="49">
+        <v>61</v>
+      </c>
+      <c r="C65" s="49">
+        <v>10</v>
+      </c>
+      <c r="D65" s="50">
+        <v>1</v>
+      </c>
+      <c r="E65" s="49">
+        <v>1</v>
+      </c>
+      <c r="F65" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G65" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H65" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="I65" s="50">
+        <v>1</v>
+      </c>
+      <c r="J65" s="49">
+        <v>1</v>
+      </c>
+      <c r="K65" s="49">
+        <v>3</v>
+      </c>
+      <c r="L65" s="51" t="s">
+        <v>616</v>
+      </c>
+      <c r="M65" s="49">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" s="52" customFormat="1">
+      <c r="A66" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B66" s="49">
+        <v>62</v>
+      </c>
+      <c r="C66" s="49">
+        <v>10</v>
+      </c>
+      <c r="D66" s="50">
+        <v>1</v>
+      </c>
+      <c r="E66" s="49">
+        <v>2</v>
+      </c>
+      <c r="F66" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G66" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H66" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="I66" s="50">
+        <v>1</v>
+      </c>
+      <c r="J66" s="49">
+        <v>1</v>
+      </c>
+      <c r="K66" s="49">
+        <v>3</v>
+      </c>
+      <c r="L66" s="51" t="s">
+        <v>618</v>
+      </c>
+      <c r="M66" s="49" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" s="52" customFormat="1">
+      <c r="A67" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B67" s="49">
+        <v>63</v>
+      </c>
+      <c r="C67" s="49">
+        <v>10</v>
+      </c>
+      <c r="D67" s="50">
+        <v>1</v>
+      </c>
+      <c r="E67" s="49">
+        <v>2</v>
+      </c>
+      <c r="F67" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G67" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H67" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="I67" s="50">
+        <v>1</v>
+      </c>
+      <c r="J67" s="49">
+        <v>1</v>
+      </c>
+      <c r="K67" s="49">
+        <v>4</v>
+      </c>
+      <c r="L67" s="51" t="s">
+        <v>618</v>
+      </c>
+      <c r="M67" s="49">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" s="52" customFormat="1">
+      <c r="A68" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B68" s="49">
+        <v>64</v>
+      </c>
+      <c r="C68" s="49">
+        <v>10</v>
+      </c>
+      <c r="D68" s="50">
+        <v>1</v>
+      </c>
+      <c r="E68" s="49">
+        <v>3</v>
+      </c>
+      <c r="F68" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G68" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H68" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="I68" s="50">
+        <v>1</v>
+      </c>
+      <c r="J68" s="49">
+        <v>1</v>
+      </c>
+      <c r="K68" s="49">
+        <v>4</v>
+      </c>
+      <c r="L68" s="51" t="s">
+        <v>618</v>
+      </c>
+      <c r="M68" s="49">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" s="52" customFormat="1">
+      <c r="A69" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B69" s="49">
+        <v>65</v>
+      </c>
+      <c r="C69" s="49">
+        <v>10</v>
+      </c>
+      <c r="D69" s="50">
+        <v>1</v>
+      </c>
+      <c r="E69" s="49">
+        <v>3</v>
+      </c>
+      <c r="F69" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G69" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H69" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="I69" s="50">
+        <v>1</v>
+      </c>
+      <c r="J69" s="49">
+        <v>1</v>
+      </c>
+      <c r="K69" s="49">
+        <v>4</v>
+      </c>
+      <c r="L69" s="51" t="s">
+        <v>618</v>
+      </c>
+      <c r="M69" s="49" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" s="52" customFormat="1">
+      <c r="A70" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B70" s="49">
+        <v>66</v>
+      </c>
+      <c r="C70" s="49">
+        <v>10</v>
+      </c>
+      <c r="D70" s="50">
+        <v>1</v>
+      </c>
+      <c r="E70" s="49">
+        <v>3</v>
+      </c>
+      <c r="F70" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G70" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H70" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="I70" s="50">
+        <v>1</v>
+      </c>
+      <c r="J70" s="49">
+        <v>1</v>
+      </c>
+      <c r="K70" s="49">
+        <v>3</v>
+      </c>
+      <c r="L70" s="51" t="s">
+        <v>620</v>
+      </c>
+      <c r="M70" s="49" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" s="52" customFormat="1" ht="30">
+      <c r="A71" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B71" s="49">
+        <v>67</v>
+      </c>
+      <c r="C71" s="49">
+        <v>10</v>
+      </c>
+      <c r="D71" s="50">
+        <v>1</v>
+      </c>
+      <c r="E71" s="49">
+        <v>1</v>
+      </c>
+      <c r="F71" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G71" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H71" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="I71" s="50">
+        <v>1</v>
+      </c>
+      <c r="J71" s="49">
+        <v>1</v>
+      </c>
+      <c r="K71" s="49">
+        <v>2</v>
+      </c>
+      <c r="L71" s="51" t="s">
+        <v>622</v>
+      </c>
+      <c r="M71" s="49" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" s="52" customFormat="1" ht="30">
+      <c r="A72" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B72" s="49">
+        <v>68</v>
+      </c>
+      <c r="C72" s="49">
+        <v>8</v>
+      </c>
+      <c r="D72" s="50">
+        <v>1</v>
+      </c>
+      <c r="E72" s="49">
+        <v>1</v>
+      </c>
+      <c r="F72" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G72" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H72" s="91" t="s">
+        <v>340</v>
+      </c>
+      <c r="I72" s="50">
+        <v>1</v>
+      </c>
+      <c r="J72" s="50">
+        <v>1</v>
+      </c>
+      <c r="K72" s="50">
+        <v>1</v>
+      </c>
+      <c r="L72" s="53" t="s">
+        <v>624</v>
+      </c>
+      <c r="M72" s="49" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" s="52" customFormat="1">
+      <c r="A73" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B73" s="49">
+        <v>69</v>
+      </c>
+      <c r="C73" s="49">
+        <v>10</v>
+      </c>
+      <c r="D73" s="50">
+        <v>1</v>
+      </c>
+      <c r="E73" s="49">
+        <v>2</v>
+      </c>
+      <c r="F73" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G73" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H73" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="I73" s="50">
+        <v>1</v>
+      </c>
+      <c r="J73" s="49">
+        <v>1</v>
+      </c>
+      <c r="K73" s="49">
+        <v>3</v>
+      </c>
+      <c r="L73" s="51" t="s">
+        <v>625</v>
+      </c>
+      <c r="M73" s="49" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" s="52" customFormat="1">
+      <c r="A74" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B74" s="49">
+        <v>70</v>
+      </c>
+      <c r="C74" s="49">
+        <v>10</v>
+      </c>
+      <c r="D74" s="50">
+        <v>1</v>
+      </c>
+      <c r="E74" s="49">
+        <v>2</v>
+      </c>
+      <c r="F74" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G74" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H74" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="I74" s="50">
+        <v>1</v>
+      </c>
+      <c r="J74" s="49">
+        <v>1</v>
+      </c>
+      <c r="K74" s="49">
+        <v>3</v>
+      </c>
+      <c r="L74" s="51" t="s">
+        <v>627</v>
+      </c>
+      <c r="M74" s="49">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" s="52" customFormat="1">
+      <c r="A75" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B75" s="49">
+        <v>71</v>
+      </c>
+      <c r="C75" s="49">
+        <v>10</v>
+      </c>
+      <c r="D75" s="50">
+        <v>1</v>
+      </c>
+      <c r="E75" s="49">
+        <v>2</v>
+      </c>
+      <c r="F75" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G75" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H75" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="I75" s="50">
+        <v>1</v>
+      </c>
+      <c r="J75" s="49">
+        <v>1</v>
+      </c>
+      <c r="K75" s="49">
+        <v>4</v>
+      </c>
+      <c r="L75" s="51" t="s">
+        <v>628</v>
+      </c>
+      <c r="M75" s="49" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" s="52" customFormat="1">
+      <c r="A76" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B76" s="49">
+        <v>72</v>
+      </c>
+      <c r="C76" s="49">
+        <v>10</v>
+      </c>
+      <c r="D76" s="50">
+        <v>1</v>
+      </c>
+      <c r="E76" s="49">
+        <v>1</v>
+      </c>
+      <c r="F76" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G76" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H76" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="I76" s="50">
+        <v>1</v>
+      </c>
+      <c r="J76" s="49">
+        <v>1</v>
+      </c>
+      <c r="K76" s="49">
+        <v>4</v>
+      </c>
+      <c r="L76" s="51" t="s">
+        <v>630</v>
+      </c>
+      <c r="M76" s="49" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" s="52" customFormat="1">
+      <c r="A77" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B77" s="49">
+        <v>73</v>
+      </c>
+      <c r="C77" s="49">
+        <v>10</v>
+      </c>
+      <c r="D77" s="50">
+        <v>1</v>
+      </c>
+      <c r="E77" s="49">
+        <v>2</v>
+      </c>
+      <c r="F77" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G77" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="H77" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="I77" s="50">
+        <v>1</v>
+      </c>
+      <c r="J77" s="49">
+        <v>1</v>
+      </c>
+      <c r="K77" s="49">
+        <v>3</v>
+      </c>
+      <c r="L77" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="M77" s="49" t="s">
+        <v>632</v>
       </c>
     </row>
   </sheetData>
@@ -36332,10 +37403,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -37053,6 +38124,88 @@
         <v>3</v>
       </c>
     </row>
+    <row r="18" spans="1:13" s="52" customFormat="1">
+      <c r="A18" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B18" s="49">
+        <v>17</v>
+      </c>
+      <c r="C18" s="49">
+        <v>10</v>
+      </c>
+      <c r="D18" s="50">
+        <v>3</v>
+      </c>
+      <c r="E18" s="49">
+        <v>1</v>
+      </c>
+      <c r="F18" s="53" t="s">
+        <v>488</v>
+      </c>
+      <c r="G18" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="H18" s="52" t="s">
+        <v>633</v>
+      </c>
+      <c r="I18" s="50">
+        <v>2</v>
+      </c>
+      <c r="J18" s="49">
+        <v>1</v>
+      </c>
+      <c r="K18" s="49">
+        <v>1</v>
+      </c>
+      <c r="L18" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18" s="49" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="52" customFormat="1">
+      <c r="A19" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B19" s="49">
+        <v>18</v>
+      </c>
+      <c r="C19" s="49">
+        <v>10</v>
+      </c>
+      <c r="D19" s="50">
+        <v>3</v>
+      </c>
+      <c r="E19" s="49">
+        <v>1</v>
+      </c>
+      <c r="F19" s="53" t="s">
+        <v>488</v>
+      </c>
+      <c r="G19" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="H19" s="52" t="s">
+        <v>633</v>
+      </c>
+      <c r="I19" s="50">
+        <v>2</v>
+      </c>
+      <c r="J19" s="49">
+        <v>1</v>
+      </c>
+      <c r="K19" s="49">
+        <v>1</v>
+      </c>
+      <c r="L19" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="49" t="s">
+        <v>635</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated questions and lists, and README
</commit_message>
<xml_diff>
--- a/lists/lists.rs.xlsx
+++ b/lists/lists.rs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="379" documentId="11_0E618F0EA1E257E00DADCD87E20241976D57A87B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EE7B453-4243-4F9B-8929-595CD33C82BB}"/>
+  <xr:revisionPtr revIDLastSave="574" documentId="11_0E618F0EA1E257E00DADCD87E20241976D57A87B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{736062A6-46AE-4C45-9E08-FDAF962B8EA4}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1476" windowWidth="15924" windowHeight="8964" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1476" windowWidth="15924" windowHeight="8964" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fractions" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3968" uniqueCount="675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4075" uniqueCount="701">
   <si>
     <t>RAZRED</t>
   </si>
@@ -2175,6 +2175,84 @@
   </si>
   <si>
     <t>rast</t>
+  </si>
+  <si>
+    <t>Realni brojevi</t>
+  </si>
+  <si>
+    <t>Iracionalni brojevi</t>
+  </si>
+  <si>
+    <t>Kvadrat racionalnog broja</t>
+  </si>
+  <si>
+    <t>numb_2 4</t>
+  </si>
+  <si>
+    <t>razlomci u raznim oblicima</t>
+  </si>
+  <si>
+    <t>tabela</t>
+  </si>
+  <si>
+    <t>upoređivanje</t>
+  </si>
+  <si>
+    <t>Kvadratni koren</t>
+  </si>
+  <si>
+    <t>pojam</t>
+  </si>
+  <si>
+    <t>Rešenje kvadratne jednačine</t>
+  </si>
+  <si>
+    <t>brojevna prava</t>
+  </si>
+  <si>
+    <t>Približna vrednost</t>
+  </si>
+  <si>
+    <t>numb_2 18, fact_2 32</t>
+  </si>
+  <si>
+    <t>Apsolutna greška</t>
+  </si>
+  <si>
+    <t>decimalni broj ili razlomak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sabiranje i oduzimanje  </t>
+  </si>
+  <si>
+    <t>zbir/razlika korena broja</t>
+  </si>
+  <si>
+    <t>fact_2 89</t>
+  </si>
+  <si>
+    <t>pojam / tabela</t>
+  </si>
+  <si>
+    <t>koren broja / tabela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poredjenje  </t>
+  </si>
+  <si>
+    <t>koren proizvoda 2 činioca istog tipa</t>
+  </si>
+  <si>
+    <t>koren proizvoda 4 činioca raznog tipa</t>
+  </si>
+  <si>
+    <t>zbir/razlika/proizvod korena brojeva</t>
+  </si>
+  <si>
+    <t>nb_2 78</t>
+  </si>
+  <si>
+    <t>nb_2 66</t>
   </si>
 </sst>
 </file>
@@ -2235,7 +2313,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2269,12 +2347,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCECFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2367,7 +2439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2656,25 +2728,16 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2683,9 +2746,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFCC"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFCCECFF"/>
       <color rgb="FFCCFFFF"/>
-      <color rgb="FFFFFFCC"/>
-      <color rgb="FFCCECFF"/>
       <color rgb="FF99FFCC"/>
       <color rgb="FFFFCCCC"/>
       <color rgb="FFFFCCFF"/>
@@ -3028,8 +3092,8 @@
   <dimension ref="A1:M69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J76" sqref="J76"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5598,10 +5662,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:M57"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7230,7 +7294,7 @@
       </c>
     </row>
     <row r="41" spans="1:13" s="18" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="120" t="s">
+      <c r="A41" s="114" t="s">
         <v>335</v>
       </c>
       <c r="B41" s="15">
@@ -7269,7 +7333,7 @@
       <c r="M41" s="15"/>
     </row>
     <row r="42" spans="1:13" s="18" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="120" t="s">
+      <c r="A42" s="114" t="s">
         <v>335</v>
       </c>
       <c r="B42" s="15">
@@ -7349,7 +7413,7 @@
       <c r="M43" s="9"/>
     </row>
     <row r="44" spans="1:13" s="18" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="120" t="s">
+      <c r="A44" s="114" t="s">
         <v>335</v>
       </c>
       <c r="B44" s="15">
@@ -7909,6 +7973,47 @@
         <v>671</v>
       </c>
       <c r="M57" s="15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="15">
+        <v>6</v>
+      </c>
+      <c r="B58" s="15">
+        <v>51</v>
+      </c>
+      <c r="C58" s="15">
+        <v>10</v>
+      </c>
+      <c r="D58" s="15">
+        <v>3</v>
+      </c>
+      <c r="E58" s="15">
+        <v>2</v>
+      </c>
+      <c r="F58" s="18" t="s">
+        <v>452</v>
+      </c>
+      <c r="G58" s="113" t="s">
+        <v>669</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>670</v>
+      </c>
+      <c r="I58" s="15">
+        <v>4</v>
+      </c>
+      <c r="J58" s="15">
+        <v>4</v>
+      </c>
+      <c r="K58" s="15">
+        <v>2</v>
+      </c>
+      <c r="L58" s="18" t="s">
+        <v>671</v>
+      </c>
+      <c r="M58" s="15">
         <v>47</v>
       </c>
     </row>
@@ -28260,10 +28365,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:M79"/>
+  <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H81" sqref="H81"/>
+    <sheetView topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31436,45 +31541,619 @@
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:13" s="119" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="114" t="s">
+    <row r="79" spans="1:13" s="52" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="90" t="s">
         <v>335</v>
       </c>
-      <c r="B79" s="115">
+      <c r="B79" s="49">
         <v>78</v>
       </c>
-      <c r="C79" s="115">
-        <v>10</v>
-      </c>
-      <c r="D79" s="116">
-        <v>2</v>
-      </c>
-      <c r="E79" s="115">
-        <v>3</v>
-      </c>
-      <c r="F79" s="117" t="s">
+      <c r="C79" s="49">
+        <v>10</v>
+      </c>
+      <c r="D79" s="50">
+        <v>2</v>
+      </c>
+      <c r="E79" s="49">
+        <v>3</v>
+      </c>
+      <c r="F79" s="53" t="s">
         <v>178</v>
       </c>
-      <c r="G79" s="118" t="s">
+      <c r="G79" s="51" t="s">
         <v>628</v>
       </c>
-      <c r="H79" s="119" t="s">
+      <c r="H79" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="I79" s="116">
-        <v>1</v>
-      </c>
-      <c r="J79" s="115">
-        <v>2</v>
-      </c>
-      <c r="K79" s="115">
-        <v>4</v>
-      </c>
-      <c r="L79" s="118" t="s">
+      <c r="I79" s="50">
+        <v>1</v>
+      </c>
+      <c r="J79" s="49">
+        <v>2</v>
+      </c>
+      <c r="K79" s="49">
+        <v>4</v>
+      </c>
+      <c r="L79" s="51" t="s">
         <v>641</v>
       </c>
-      <c r="M79" s="115">
+      <c r="M79" s="49">
         <v>73</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" s="116" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="116">
+        <v>7</v>
+      </c>
+      <c r="B80" s="116">
+        <v>79</v>
+      </c>
+      <c r="C80" s="116">
+        <v>10</v>
+      </c>
+      <c r="D80" s="116">
+        <v>1</v>
+      </c>
+      <c r="E80" s="116">
+        <v>1</v>
+      </c>
+      <c r="F80" s="115" t="s">
+        <v>675</v>
+      </c>
+      <c r="G80" s="115" t="s">
+        <v>676</v>
+      </c>
+      <c r="H80" s="115" t="s">
+        <v>677</v>
+      </c>
+      <c r="I80" s="116">
+        <v>1</v>
+      </c>
+      <c r="J80" s="116">
+        <v>1</v>
+      </c>
+      <c r="K80" s="116">
+        <v>1</v>
+      </c>
+      <c r="L80" s="115" t="s">
+        <v>680</v>
+      </c>
+      <c r="M80" s="116">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" s="116" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="116">
+        <v>7</v>
+      </c>
+      <c r="B81" s="116">
+        <v>80</v>
+      </c>
+      <c r="C81" s="116">
+        <v>10</v>
+      </c>
+      <c r="D81" s="116">
+        <v>1</v>
+      </c>
+      <c r="E81" s="116">
+        <v>2</v>
+      </c>
+      <c r="F81" s="115" t="s">
+        <v>675</v>
+      </c>
+      <c r="G81" s="115" t="s">
+        <v>676</v>
+      </c>
+      <c r="H81" s="115" t="s">
+        <v>677</v>
+      </c>
+      <c r="I81" s="116">
+        <v>1</v>
+      </c>
+      <c r="J81" s="116">
+        <v>1</v>
+      </c>
+      <c r="K81" s="116">
+        <v>1</v>
+      </c>
+      <c r="L81" s="115" t="s">
+        <v>679</v>
+      </c>
+      <c r="M81" s="116">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" s="116" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="116">
+        <v>7</v>
+      </c>
+      <c r="B82" s="116">
+        <v>81</v>
+      </c>
+      <c r="C82" s="116">
+        <v>10</v>
+      </c>
+      <c r="D82" s="116">
+        <v>1</v>
+      </c>
+      <c r="E82" s="116">
+        <v>2</v>
+      </c>
+      <c r="F82" s="115" t="s">
+        <v>675</v>
+      </c>
+      <c r="G82" s="115" t="s">
+        <v>676</v>
+      </c>
+      <c r="H82" s="115" t="s">
+        <v>677</v>
+      </c>
+      <c r="I82" s="116">
+        <v>1</v>
+      </c>
+      <c r="J82" s="116">
+        <v>1</v>
+      </c>
+      <c r="K82" s="116">
+        <v>1</v>
+      </c>
+      <c r="L82" s="115" t="s">
+        <v>442</v>
+      </c>
+      <c r="M82" s="116">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" s="116" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="116">
+        <v>7</v>
+      </c>
+      <c r="B83" s="116">
+        <v>82</v>
+      </c>
+      <c r="C83" s="116">
+        <v>10</v>
+      </c>
+      <c r="D83" s="116">
+        <v>1</v>
+      </c>
+      <c r="E83" s="116">
+        <v>1</v>
+      </c>
+      <c r="F83" s="115" t="s">
+        <v>675</v>
+      </c>
+      <c r="G83" s="115" t="s">
+        <v>676</v>
+      </c>
+      <c r="H83" s="115" t="s">
+        <v>677</v>
+      </c>
+      <c r="I83" s="116">
+        <v>1</v>
+      </c>
+      <c r="J83" s="116">
+        <v>1</v>
+      </c>
+      <c r="K83" s="116">
+        <v>1</v>
+      </c>
+      <c r="L83" s="115" t="s">
+        <v>681</v>
+      </c>
+      <c r="M83" s="116">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" s="116" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="116">
+        <v>7</v>
+      </c>
+      <c r="B84" s="116">
+        <v>83</v>
+      </c>
+      <c r="C84" s="116">
+        <v>10</v>
+      </c>
+      <c r="D84" s="116">
+        <v>1</v>
+      </c>
+      <c r="E84" s="116">
+        <v>1</v>
+      </c>
+      <c r="F84" s="115" t="s">
+        <v>675</v>
+      </c>
+      <c r="G84" s="115" t="s">
+        <v>676</v>
+      </c>
+      <c r="H84" s="115" t="s">
+        <v>677</v>
+      </c>
+      <c r="I84" s="116">
+        <v>1</v>
+      </c>
+      <c r="J84" s="116">
+        <v>1</v>
+      </c>
+      <c r="K84" s="116">
+        <v>1</v>
+      </c>
+      <c r="L84" s="115" t="s">
+        <v>442</v>
+      </c>
+      <c r="M84" s="116">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" s="116" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="116">
+        <v>7</v>
+      </c>
+      <c r="B85" s="116">
+        <v>84</v>
+      </c>
+      <c r="C85" s="116">
+        <v>10</v>
+      </c>
+      <c r="D85" s="116">
+        <v>1</v>
+      </c>
+      <c r="E85" s="116">
+        <v>1</v>
+      </c>
+      <c r="F85" s="115" t="s">
+        <v>675</v>
+      </c>
+      <c r="G85" s="115" t="s">
+        <v>676</v>
+      </c>
+      <c r="H85" s="115" t="s">
+        <v>682</v>
+      </c>
+      <c r="I85" s="116">
+        <v>1</v>
+      </c>
+      <c r="J85" s="116">
+        <v>1</v>
+      </c>
+      <c r="K85" s="116">
+        <v>2</v>
+      </c>
+      <c r="L85" s="115" t="s">
+        <v>693</v>
+      </c>
+      <c r="M85" s="116">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" s="116" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="116">
+        <v>7</v>
+      </c>
+      <c r="B86" s="116">
+        <v>85</v>
+      </c>
+      <c r="C86" s="116">
+        <v>10</v>
+      </c>
+      <c r="D86" s="116">
+        <v>1</v>
+      </c>
+      <c r="E86" s="116">
+        <v>2</v>
+      </c>
+      <c r="F86" s="115" t="s">
+        <v>675</v>
+      </c>
+      <c r="G86" s="115" t="s">
+        <v>676</v>
+      </c>
+      <c r="H86" s="115" t="s">
+        <v>682</v>
+      </c>
+      <c r="I86" s="116">
+        <v>1</v>
+      </c>
+      <c r="J86" s="116">
+        <v>1</v>
+      </c>
+      <c r="K86" s="116">
+        <v>2</v>
+      </c>
+      <c r="L86" s="63" t="s">
+        <v>684</v>
+      </c>
+      <c r="M86" s="116">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" s="116" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="116">
+        <v>7</v>
+      </c>
+      <c r="B87" s="116">
+        <v>86</v>
+      </c>
+      <c r="C87" s="116">
+        <v>10</v>
+      </c>
+      <c r="D87" s="116">
+        <v>1</v>
+      </c>
+      <c r="E87" s="116">
+        <v>2</v>
+      </c>
+      <c r="F87" s="115" t="s">
+        <v>675</v>
+      </c>
+      <c r="G87" s="115" t="s">
+        <v>676</v>
+      </c>
+      <c r="H87" s="115" t="s">
+        <v>682</v>
+      </c>
+      <c r="I87" s="116">
+        <v>1</v>
+      </c>
+      <c r="J87" s="116">
+        <v>1</v>
+      </c>
+      <c r="K87" s="116">
+        <v>2</v>
+      </c>
+      <c r="L87" s="63" t="s">
+        <v>684</v>
+      </c>
+      <c r="M87" s="116">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" s="116" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="116">
+        <v>7</v>
+      </c>
+      <c r="B88" s="116">
+        <v>87</v>
+      </c>
+      <c r="C88" s="116">
+        <v>10</v>
+      </c>
+      <c r="D88" s="116">
+        <v>1</v>
+      </c>
+      <c r="E88" s="116">
+        <v>3</v>
+      </c>
+      <c r="F88" s="115" t="s">
+        <v>675</v>
+      </c>
+      <c r="G88" s="115" t="s">
+        <v>676</v>
+      </c>
+      <c r="H88" s="115" t="s">
+        <v>682</v>
+      </c>
+      <c r="I88" s="116">
+        <v>1</v>
+      </c>
+      <c r="J88" s="116">
+        <v>1</v>
+      </c>
+      <c r="K88" s="116">
+        <v>2</v>
+      </c>
+      <c r="L88" s="63" t="s">
+        <v>684</v>
+      </c>
+      <c r="M88" s="116">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" s="116" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="116">
+        <v>7</v>
+      </c>
+      <c r="B89" s="116">
+        <v>88</v>
+      </c>
+      <c r="C89" s="116">
+        <v>10</v>
+      </c>
+      <c r="D89" s="116">
+        <v>1</v>
+      </c>
+      <c r="E89" s="116">
+        <v>1</v>
+      </c>
+      <c r="F89" s="115" t="s">
+        <v>675</v>
+      </c>
+      <c r="G89" s="115" t="s">
+        <v>676</v>
+      </c>
+      <c r="H89" s="115" t="s">
+        <v>682</v>
+      </c>
+      <c r="I89" s="116">
+        <v>1</v>
+      </c>
+      <c r="J89" s="116">
+        <v>1</v>
+      </c>
+      <c r="K89" s="116">
+        <v>2</v>
+      </c>
+      <c r="L89" s="115" t="s">
+        <v>683</v>
+      </c>
+      <c r="M89" s="116">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" s="116" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="116">
+        <v>7</v>
+      </c>
+      <c r="B90" s="116">
+        <v>89</v>
+      </c>
+      <c r="C90" s="116">
+        <v>10</v>
+      </c>
+      <c r="D90" s="116">
+        <v>1</v>
+      </c>
+      <c r="E90" s="116">
+        <v>2</v>
+      </c>
+      <c r="F90" s="115" t="s">
+        <v>675</v>
+      </c>
+      <c r="G90" s="115" t="s">
+        <v>676</v>
+      </c>
+      <c r="H90" s="115" t="s">
+        <v>682</v>
+      </c>
+      <c r="I90" s="116">
+        <v>1</v>
+      </c>
+      <c r="J90" s="116">
+        <v>1</v>
+      </c>
+      <c r="K90" s="116">
+        <v>2</v>
+      </c>
+      <c r="L90" s="115" t="s">
+        <v>683</v>
+      </c>
+      <c r="M90" s="116">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" s="116" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="116">
+        <v>7</v>
+      </c>
+      <c r="B91" s="116">
+        <v>90</v>
+      </c>
+      <c r="C91" s="116">
+        <v>10</v>
+      </c>
+      <c r="D91" s="116">
+        <v>1</v>
+      </c>
+      <c r="E91" s="116">
+        <v>1</v>
+      </c>
+      <c r="F91" s="115" t="s">
+        <v>675</v>
+      </c>
+      <c r="G91" s="115" t="s">
+        <v>676</v>
+      </c>
+      <c r="H91" s="115" t="s">
+        <v>682</v>
+      </c>
+      <c r="I91" s="116">
+        <v>1</v>
+      </c>
+      <c r="J91" s="116">
+        <v>1</v>
+      </c>
+      <c r="K91" s="116">
+        <v>2</v>
+      </c>
+      <c r="L91" s="115" t="s">
+        <v>685</v>
+      </c>
+      <c r="M91" s="116">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" s="116" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="116">
+        <v>7</v>
+      </c>
+      <c r="B92" s="116">
+        <v>91</v>
+      </c>
+      <c r="C92" s="116">
+        <v>10</v>
+      </c>
+      <c r="D92" s="116">
+        <v>1</v>
+      </c>
+      <c r="E92" s="116">
+        <v>1</v>
+      </c>
+      <c r="F92" s="115" t="s">
+        <v>675</v>
+      </c>
+      <c r="G92" s="115" t="s">
+        <v>125</v>
+      </c>
+      <c r="H92" s="115" t="s">
+        <v>150</v>
+      </c>
+      <c r="I92" s="116">
+        <v>1</v>
+      </c>
+      <c r="J92" s="116">
+        <v>3</v>
+      </c>
+      <c r="K92" s="116">
+        <v>2</v>
+      </c>
+      <c r="L92" s="115" t="s">
+        <v>696</v>
+      </c>
+      <c r="M92" s="116">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" s="116" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="116">
+        <v>7</v>
+      </c>
+      <c r="B93" s="116">
+        <v>92</v>
+      </c>
+      <c r="C93" s="116">
+        <v>10</v>
+      </c>
+      <c r="D93" s="116">
+        <v>1</v>
+      </c>
+      <c r="E93" s="116">
+        <v>2</v>
+      </c>
+      <c r="F93" s="115" t="s">
+        <v>675</v>
+      </c>
+      <c r="G93" s="115" t="s">
+        <v>125</v>
+      </c>
+      <c r="H93" s="115" t="s">
+        <v>150</v>
+      </c>
+      <c r="I93" s="116">
+        <v>1</v>
+      </c>
+      <c r="J93" s="116">
+        <v>3</v>
+      </c>
+      <c r="K93" s="116">
+        <v>2</v>
+      </c>
+      <c r="L93" s="115" t="s">
+        <v>697</v>
+      </c>
+      <c r="M93" s="116">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -31487,7 +32166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+    <sheetView topLeftCell="G97" workbookViewId="0">
       <selection activeCell="M103" sqref="M103"/>
     </sheetView>
   </sheetViews>
@@ -35865,10 +36544,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:N77"/>
+  <dimension ref="A1:N87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A77" sqref="A77:XFD77"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="M87" sqref="M87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38982,6 +39661,414 @@
       </c>
       <c r="M77" s="49" t="s">
         <v>624</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="116">
+        <v>7</v>
+      </c>
+      <c r="B78" s="34">
+        <v>74</v>
+      </c>
+      <c r="C78" s="34">
+        <v>10</v>
+      </c>
+      <c r="D78" s="35">
+        <v>1</v>
+      </c>
+      <c r="E78" s="34">
+        <v>1</v>
+      </c>
+      <c r="F78" s="117" t="s">
+        <v>675</v>
+      </c>
+      <c r="G78" s="117" t="s">
+        <v>676</v>
+      </c>
+      <c r="H78" s="117" t="s">
+        <v>677</v>
+      </c>
+      <c r="I78" s="116">
+        <v>1</v>
+      </c>
+      <c r="J78" s="116">
+        <v>1</v>
+      </c>
+      <c r="K78" s="116">
+        <v>1</v>
+      </c>
+      <c r="L78" s="38" t="s">
+        <v>695</v>
+      </c>
+      <c r="M78" s="116" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="116">
+        <v>7</v>
+      </c>
+      <c r="B79" s="34">
+        <v>75</v>
+      </c>
+      <c r="C79" s="34">
+        <v>10</v>
+      </c>
+      <c r="D79" s="35">
+        <v>1</v>
+      </c>
+      <c r="E79" s="34">
+        <v>1</v>
+      </c>
+      <c r="F79" s="117" t="s">
+        <v>675</v>
+      </c>
+      <c r="G79" s="117" t="s">
+        <v>676</v>
+      </c>
+      <c r="H79" s="117" t="s">
+        <v>682</v>
+      </c>
+      <c r="I79" s="116">
+        <v>1</v>
+      </c>
+      <c r="J79" s="116">
+        <v>1</v>
+      </c>
+      <c r="K79" s="116">
+        <v>2</v>
+      </c>
+      <c r="L79" s="38" t="s">
+        <v>374</v>
+      </c>
+      <c r="M79" s="116" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="116">
+        <v>7</v>
+      </c>
+      <c r="B80" s="34">
+        <v>76</v>
+      </c>
+      <c r="C80" s="34">
+        <v>10</v>
+      </c>
+      <c r="D80" s="35">
+        <v>1</v>
+      </c>
+      <c r="E80" s="34">
+        <v>1</v>
+      </c>
+      <c r="F80" s="117" t="s">
+        <v>675</v>
+      </c>
+      <c r="G80" s="117" t="s">
+        <v>403</v>
+      </c>
+      <c r="H80" s="117" t="s">
+        <v>686</v>
+      </c>
+      <c r="I80" s="116">
+        <v>1</v>
+      </c>
+      <c r="J80" s="116">
+        <v>2</v>
+      </c>
+      <c r="K80" s="116">
+        <v>1</v>
+      </c>
+      <c r="L80" s="38" t="s">
+        <v>689</v>
+      </c>
+      <c r="M80" s="116" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="116">
+        <v>7</v>
+      </c>
+      <c r="B81" s="34">
+        <v>76</v>
+      </c>
+      <c r="C81" s="34">
+        <v>10</v>
+      </c>
+      <c r="D81" s="35">
+        <v>1</v>
+      </c>
+      <c r="E81" s="34">
+        <v>1</v>
+      </c>
+      <c r="F81" s="117" t="s">
+        <v>675</v>
+      </c>
+      <c r="G81" s="117" t="s">
+        <v>403</v>
+      </c>
+      <c r="H81" s="117" t="s">
+        <v>688</v>
+      </c>
+      <c r="I81" s="116">
+        <v>1</v>
+      </c>
+      <c r="J81" s="116">
+        <v>2</v>
+      </c>
+      <c r="K81" s="116">
+        <v>2</v>
+      </c>
+      <c r="L81" s="38" t="s">
+        <v>689</v>
+      </c>
+      <c r="M81" s="116" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="116">
+        <v>7</v>
+      </c>
+      <c r="B82" s="34">
+        <v>77</v>
+      </c>
+      <c r="C82" s="34">
+        <v>10</v>
+      </c>
+      <c r="D82" s="35">
+        <v>1</v>
+      </c>
+      <c r="E82" s="34">
+        <v>2</v>
+      </c>
+      <c r="F82" s="117" t="s">
+        <v>675</v>
+      </c>
+      <c r="G82" s="117" t="s">
+        <v>403</v>
+      </c>
+      <c r="H82" s="117" t="s">
+        <v>686</v>
+      </c>
+      <c r="I82" s="116">
+        <v>1</v>
+      </c>
+      <c r="J82" s="116">
+        <v>2</v>
+      </c>
+      <c r="K82" s="116">
+        <v>1</v>
+      </c>
+      <c r="L82" s="38" t="s">
+        <v>694</v>
+      </c>
+      <c r="M82" s="116">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="116">
+        <v>7</v>
+      </c>
+      <c r="B83" s="34">
+        <v>77</v>
+      </c>
+      <c r="C83" s="34">
+        <v>10</v>
+      </c>
+      <c r="D83" s="35">
+        <v>1</v>
+      </c>
+      <c r="E83" s="34">
+        <v>2</v>
+      </c>
+      <c r="F83" s="117" t="s">
+        <v>675</v>
+      </c>
+      <c r="G83" s="117" t="s">
+        <v>403</v>
+      </c>
+      <c r="H83" s="117" t="s">
+        <v>688</v>
+      </c>
+      <c r="I83" s="116">
+        <v>1</v>
+      </c>
+      <c r="J83" s="116">
+        <v>2</v>
+      </c>
+      <c r="K83" s="116">
+        <v>2</v>
+      </c>
+      <c r="L83" s="38" t="s">
+        <v>694</v>
+      </c>
+      <c r="M83" s="116">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="116">
+        <v>7</v>
+      </c>
+      <c r="B84" s="34">
+        <v>78</v>
+      </c>
+      <c r="C84" s="34">
+        <v>10</v>
+      </c>
+      <c r="D84" s="35">
+        <v>1</v>
+      </c>
+      <c r="E84" s="34">
+        <v>2</v>
+      </c>
+      <c r="F84" s="117" t="s">
+        <v>675</v>
+      </c>
+      <c r="G84" s="117" t="s">
+        <v>125</v>
+      </c>
+      <c r="H84" s="117" t="s">
+        <v>690</v>
+      </c>
+      <c r="I84" s="116">
+        <v>1</v>
+      </c>
+      <c r="J84" s="116">
+        <v>3</v>
+      </c>
+      <c r="K84" s="116">
+        <v>1</v>
+      </c>
+      <c r="L84" s="38" t="s">
+        <v>691</v>
+      </c>
+      <c r="M84" s="116" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="116">
+        <v>7</v>
+      </c>
+      <c r="B85" s="34">
+        <v>79</v>
+      </c>
+      <c r="C85" s="34">
+        <v>10</v>
+      </c>
+      <c r="D85" s="35">
+        <v>1</v>
+      </c>
+      <c r="E85" s="34">
+        <v>2</v>
+      </c>
+      <c r="F85" s="117" t="s">
+        <v>675</v>
+      </c>
+      <c r="G85" s="117" t="s">
+        <v>125</v>
+      </c>
+      <c r="H85" s="117" t="s">
+        <v>690</v>
+      </c>
+      <c r="I85" s="116">
+        <v>1</v>
+      </c>
+      <c r="J85" s="116">
+        <v>3</v>
+      </c>
+      <c r="K85" s="116">
+        <v>1</v>
+      </c>
+      <c r="L85" s="38" t="s">
+        <v>691</v>
+      </c>
+      <c r="M85" s="116"/>
+    </row>
+    <row r="86" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="116">
+        <v>7</v>
+      </c>
+      <c r="B86" s="34">
+        <v>80</v>
+      </c>
+      <c r="C86" s="34">
+        <v>10</v>
+      </c>
+      <c r="D86" s="35">
+        <v>1</v>
+      </c>
+      <c r="E86" s="34">
+        <v>2</v>
+      </c>
+      <c r="F86" s="117" t="s">
+        <v>675</v>
+      </c>
+      <c r="G86" s="117" t="s">
+        <v>125</v>
+      </c>
+      <c r="H86" s="117" t="s">
+        <v>75</v>
+      </c>
+      <c r="I86" s="116">
+        <v>1</v>
+      </c>
+      <c r="J86" s="116">
+        <v>3</v>
+      </c>
+      <c r="K86" s="116">
+        <v>3</v>
+      </c>
+      <c r="L86" s="38" t="s">
+        <v>698</v>
+      </c>
+      <c r="M86" s="116" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="116">
+        <v>7</v>
+      </c>
+      <c r="B87" s="34">
+        <v>81</v>
+      </c>
+      <c r="C87" s="34">
+        <v>10</v>
+      </c>
+      <c r="D87" s="35">
+        <v>1</v>
+      </c>
+      <c r="E87" s="34">
+        <v>2</v>
+      </c>
+      <c r="F87" s="117" t="s">
+        <v>675</v>
+      </c>
+      <c r="G87" s="117" t="s">
+        <v>125</v>
+      </c>
+      <c r="H87" s="117" t="s">
+        <v>75</v>
+      </c>
+      <c r="I87" s="116">
+        <v>1</v>
+      </c>
+      <c r="J87" s="116">
+        <v>3</v>
+      </c>
+      <c r="K87" s="116">
+        <v>3</v>
+      </c>
+      <c r="L87" s="38" t="s">
+        <v>698</v>
+      </c>
+      <c r="M87" s="116" t="s">
+        <v>700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>